<commit_message>
HW2 - Final Challenge - Tuesday night submit
</commit_message>
<xml_diff>
--- a/Working/HW2_Working/Homogenous/HW2_Noonan-Working_Homogeneous.xlsx
+++ b/Working/HW2_Working/Homogenous/HW2_Noonan-Working_Homogeneous.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\HWRS_582\hw-genoonan\Working\HW2_Working\Homogenous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074C6741-4CBA-497C-ABAA-2F9D017CA41E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E2C4B0-1B61-4A6F-B1F3-9AA1B6A4BF47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{1D99F772-0D8B-4E27-973E-8346F0B8FA0B}"/>
   </bookViews>
@@ -11188,76 +11188,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.9999999999999931E-3</c:v>
+                  <c:v>1.9999999999999931E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.9999999999999931E-3</c:v>
+                  <c:v>1.9999999999999931E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.9999999999999931E-3</c:v>
+                  <c:v>1.9999999999999931E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.9999999999999931E-3</c:v>
+                  <c:v>1.9999999999999931E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-2.0999999999999908E-3</c:v>
+                  <c:v>2.0999999999999908E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-2.1000000000000085E-3</c:v>
+                  <c:v>2.1000000000000085E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11308,8 +11308,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -11340,8 +11341,8 @@
         <c:axId val="309901712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0"/>
-          <c:min val="-4.000000000000001E-3"/>
+          <c:max val="3.0000000000000009E-3"/>
+          <c:min val="1.0000000000000002E-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -12691,16 +12692,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23921,7 +23922,7 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="B2" sqref="B2:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24017,104 +24018,104 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <f>-1*'K values'!A1*((Head!A1)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A1)+(1/'K values'!A1)))*((Head!A1-Head!A1)/100))</f>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f>'K values'!B1*((Head!B1-Head!A1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B1)+(1/'K values'!A1)))*((Head!B1-Head!A1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D2" s="1">
-        <f>'K values'!C1*((Head!C1-Head!B1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C1)+(1/'K values'!B1)))*((Head!C1-Head!B1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E2" s="1">
-        <f>'K values'!D1*((Head!D1-Head!C1)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D1)+(1/'K values'!C1)))*((Head!D1-Head!C1)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F2" s="1">
-        <f>'K values'!E1*((Head!E1-Head!D1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E1)+(1/'K values'!D1)))*((Head!E1-Head!D1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G2" s="1">
-        <f>'K values'!F1*((Head!F1-Head!E1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F1)+(1/'K values'!E1)))*((Head!F1-Head!E1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H2" s="1">
-        <f>'K values'!G1*((Head!G1-Head!F1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G1)+(1/'K values'!F1)))*((Head!G1-Head!F1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I2" s="1">
-        <f>'K values'!H1*((Head!H1-Head!G1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H1)+(1/'K values'!G1)))*((Head!H1-Head!G1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J2" s="1">
-        <f>'K values'!I1*((Head!I1-Head!H1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I1)+(1/'K values'!H1)))*((Head!I1-Head!H1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K2" s="1">
-        <f>'K values'!J1*((Head!J1-Head!I1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J1)+(1/'K values'!I1)))*((Head!J1-Head!I1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L2" s="1">
-        <f>'K values'!K1*((Head!K1-Head!J1)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K1)+(1/'K values'!J1)))*((Head!K1-Head!J1)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M2" s="1">
-        <f>'K values'!L1*((Head!L1-Head!K1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L1)+(1/'K values'!K1)))*((Head!L1-Head!K1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N2" s="1">
-        <f>'K values'!M1*((Head!M1-Head!L1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M1)+(1/'K values'!L1)))*((Head!M1-Head!L1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O2" s="1">
-        <f>'K values'!N1*((Head!N1-Head!M1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N1)+(1/'K values'!M1)))*((Head!N1-Head!M1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P2" s="1">
-        <f>'K values'!O1*((Head!O1-Head!N1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O1)+(1/'K values'!N1)))*((Head!O1-Head!N1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q2" s="1">
-        <f>'K values'!P1*((Head!P1-Head!O1)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P1)+(1/'K values'!O1)))*((Head!P1-Head!O1)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R2" s="1">
-        <f>'K values'!Q1*((Head!Q1-Head!P1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q1)+(1/'K values'!P1)))*((Head!Q1-Head!P1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S2" s="1">
-        <f>'K values'!R1*((Head!R1-Head!Q1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R1)+(1/'K values'!Q1)))*((Head!R1-Head!Q1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T2" s="1">
-        <f>'K values'!S1*((Head!S1-Head!R1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S1)+(1/'K values'!R1)))*((Head!S1-Head!R1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U2" s="1">
-        <f>'K values'!T1*((Head!T1-Head!S1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T1)+(1/'K values'!S1)))*((Head!T1-Head!S1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V2" s="1">
-        <f>'K values'!U1*((Head!U1-Head!T1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U1)+(1/'K values'!T1)))*((Head!U1-Head!T1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W2" s="1">
-        <f>'K values'!V1*((Head!V1-Head!U1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V1)+(1/'K values'!U1)))*((Head!V1-Head!U1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X2" s="1">
-        <f>'K values'!W1*((Head!W1-Head!V1)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W1)+(1/'K values'!V1)))*((Head!W1-Head!V1)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y2" s="1">
-        <f>'K values'!X1*((Head!X1-Head!W1)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X1)+(1/'K values'!W1)))*((Head!X1-Head!W1)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z2" s="1">
-        <f>'K values'!Y1*((Head!Y1-Head!X1)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y1)+(1/'K values'!X1)))*((Head!Y1-Head!X1)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -24125,104 +24126,104 @@
         <v>100</v>
       </c>
       <c r="B3" s="1">
-        <f>-1*'K values'!A2*((Head!A2)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A2)+(1/'K values'!A2)))*((Head!A2-Head!A2)/100))</f>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <f>'K values'!B2*((Head!B2-Head!A2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B2)+(1/'K values'!A2)))*((Head!B2-Head!A2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D3" s="1">
-        <f>'K values'!C2*((Head!C2-Head!B2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C2)+(1/'K values'!B2)))*((Head!C2-Head!B2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E3" s="1">
-        <f>'K values'!D2*((Head!D2-Head!C2)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D2)+(1/'K values'!C2)))*((Head!D2-Head!C2)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F3" s="1">
-        <f>'K values'!E2*((Head!E2-Head!D2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E2)+(1/'K values'!D2)))*((Head!E2-Head!D2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G3" s="1">
-        <f>'K values'!F2*((Head!F2-Head!E2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F2)+(1/'K values'!E2)))*((Head!F2-Head!E2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H3" s="1">
-        <f>'K values'!G2*((Head!G2-Head!F2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G2)+(1/'K values'!F2)))*((Head!G2-Head!F2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I3" s="1">
-        <f>'K values'!H2*((Head!H2-Head!G2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H2)+(1/'K values'!G2)))*((Head!H2-Head!G2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J3" s="1">
-        <f>'K values'!I2*((Head!I2-Head!H2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I2)+(1/'K values'!H2)))*((Head!I2-Head!H2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K3" s="1">
-        <f>'K values'!J2*((Head!J2-Head!I2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J2)+(1/'K values'!I2)))*((Head!J2-Head!I2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L3" s="1">
-        <f>'K values'!K2*((Head!K2-Head!J2)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K2)+(1/'K values'!J2)))*((Head!K2-Head!J2)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M3" s="1">
-        <f>'K values'!L2*((Head!L2-Head!K2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L2)+(1/'K values'!K2)))*((Head!L2-Head!K2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N3" s="1">
-        <f>'K values'!M2*((Head!M2-Head!L2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M2)+(1/'K values'!L2)))*((Head!M2-Head!L2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O3" s="1">
-        <f>'K values'!N2*((Head!N2-Head!M2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N2)+(1/'K values'!M2)))*((Head!N2-Head!M2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P3" s="1">
-        <f>'K values'!O2*((Head!O2-Head!N2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O2)+(1/'K values'!N2)))*((Head!O2-Head!N2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q3" s="1">
-        <f>'K values'!P2*((Head!P2-Head!O2)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P2)+(1/'K values'!O2)))*((Head!P2-Head!O2)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R3" s="1">
-        <f>'K values'!Q2*((Head!Q2-Head!P2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q2)+(1/'K values'!P2)))*((Head!Q2-Head!P2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S3" s="1">
-        <f>'K values'!R2*((Head!R2-Head!Q2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R2)+(1/'K values'!Q2)))*((Head!R2-Head!Q2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T3" s="1">
-        <f>'K values'!S2*((Head!S2-Head!R2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S2)+(1/'K values'!R2)))*((Head!S2-Head!R2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U3" s="1">
-        <f>'K values'!T2*((Head!T2-Head!S2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T2)+(1/'K values'!S2)))*((Head!T2-Head!S2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V3" s="1">
-        <f>'K values'!U2*((Head!U2-Head!T2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U2)+(1/'K values'!T2)))*((Head!U2-Head!T2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W3" s="1">
-        <f>'K values'!V2*((Head!V2-Head!U2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V2)+(1/'K values'!U2)))*((Head!V2-Head!U2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X3" s="1">
-        <f>'K values'!W2*((Head!W2-Head!V2)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W2)+(1/'K values'!V2)))*((Head!W2-Head!V2)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y3" s="1">
-        <f>'K values'!X2*((Head!X2-Head!W2)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X2)+(1/'K values'!W2)))*((Head!X2-Head!W2)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z3" s="1">
-        <f>'K values'!Y2*((Head!Y2-Head!X2)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y2)+(1/'K values'!X2)))*((Head!Y2-Head!X2)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA3">
         <v>100</v>
@@ -24233,104 +24234,104 @@
         <v>200</v>
       </c>
       <c r="B4" s="1">
-        <f>-1*'K values'!A3*((Head!A3)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A3)+(1/'K values'!A3)))*((Head!A3-Head!A3)/100))</f>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f>'K values'!B3*((Head!B3-Head!A3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B3)+(1/'K values'!A3)))*((Head!B3-Head!A3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D4" s="1">
-        <f>'K values'!C3*((Head!C3-Head!B3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C3)+(1/'K values'!B3)))*((Head!C3-Head!B3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E4" s="1">
-        <f>'K values'!D3*((Head!D3-Head!C3)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D3)+(1/'K values'!C3)))*((Head!D3-Head!C3)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F4" s="1">
-        <f>'K values'!E3*((Head!E3-Head!D3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E3)+(1/'K values'!D3)))*((Head!E3-Head!D3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G4" s="1">
-        <f>'K values'!F3*((Head!F3-Head!E3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F3)+(1/'K values'!E3)))*((Head!F3-Head!E3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H4" s="1">
-        <f>'K values'!G3*((Head!G3-Head!F3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G3)+(1/'K values'!F3)))*((Head!G3-Head!F3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I4" s="1">
-        <f>'K values'!H3*((Head!H3-Head!G3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H3)+(1/'K values'!G3)))*((Head!H3-Head!G3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J4" s="1">
-        <f>'K values'!I3*((Head!I3-Head!H3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I3)+(1/'K values'!H3)))*((Head!I3-Head!H3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K4" s="1">
-        <f>'K values'!J3*((Head!J3-Head!I3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J3)+(1/'K values'!I3)))*((Head!J3-Head!I3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L4" s="1">
-        <f>'K values'!K3*((Head!K3-Head!J3)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K3)+(1/'K values'!J3)))*((Head!K3-Head!J3)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M4" s="1">
-        <f>'K values'!L3*((Head!L3-Head!K3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L3)+(1/'K values'!K3)))*((Head!L3-Head!K3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N4" s="1">
-        <f>'K values'!M3*((Head!M3-Head!L3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M3)+(1/'K values'!L3)))*((Head!M3-Head!L3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O4" s="1">
-        <f>'K values'!N3*((Head!N3-Head!M3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N3)+(1/'K values'!M3)))*((Head!N3-Head!M3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P4" s="1">
-        <f>'K values'!O3*((Head!O3-Head!N3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O3)+(1/'K values'!N3)))*((Head!O3-Head!N3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q4" s="1">
-        <f>'K values'!P3*((Head!P3-Head!O3)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P3)+(1/'K values'!O3)))*((Head!P3-Head!O3)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R4" s="1">
-        <f>'K values'!Q3*((Head!Q3-Head!P3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q3)+(1/'K values'!P3)))*((Head!Q3-Head!P3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S4" s="1">
-        <f>'K values'!R3*((Head!R3-Head!Q3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R3)+(1/'K values'!Q3)))*((Head!R3-Head!Q3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T4" s="1">
-        <f>'K values'!S3*((Head!S3-Head!R3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S3)+(1/'K values'!R3)))*((Head!S3-Head!R3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U4" s="1">
-        <f>'K values'!T3*((Head!T3-Head!S3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T3)+(1/'K values'!S3)))*((Head!T3-Head!S3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V4" s="1">
-        <f>'K values'!U3*((Head!U3-Head!T3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U3)+(1/'K values'!T3)))*((Head!U3-Head!T3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W4" s="1">
-        <f>'K values'!V3*((Head!V3-Head!U3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V3)+(1/'K values'!U3)))*((Head!V3-Head!U3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X4" s="1">
-        <f>'K values'!W3*((Head!W3-Head!V3)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W3)+(1/'K values'!V3)))*((Head!W3-Head!V3)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y4" s="1">
-        <f>'K values'!X3*((Head!X3-Head!W3)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X3)+(1/'K values'!W3)))*((Head!X3-Head!W3)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z4" s="1">
-        <f>'K values'!Y3*((Head!Y3-Head!X3)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y3)+(1/'K values'!X3)))*((Head!Y3-Head!X3)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA4">
         <v>200</v>
@@ -24341,104 +24342,104 @@
         <v>300</v>
       </c>
       <c r="B5" s="1">
-        <f>-1*'K values'!A4*((Head!A4)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A4)+(1/'K values'!A4)))*((Head!A4-Head!A4)/100))</f>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <f>'K values'!B4*((Head!B4-Head!A4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B4)+(1/'K values'!A4)))*((Head!B4-Head!A4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D5" s="1">
-        <f>'K values'!C4*((Head!C4-Head!B4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C4)+(1/'K values'!B4)))*((Head!C4-Head!B4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E5" s="1">
-        <f>'K values'!D4*((Head!D4-Head!C4)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D4)+(1/'K values'!C4)))*((Head!D4-Head!C4)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F5" s="1">
-        <f>'K values'!E4*((Head!E4-Head!D4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E4)+(1/'K values'!D4)))*((Head!E4-Head!D4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G5" s="1">
-        <f>'K values'!F4*((Head!F4-Head!E4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F4)+(1/'K values'!E4)))*((Head!F4-Head!E4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H5" s="1">
-        <f>'K values'!G4*((Head!G4-Head!F4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G4)+(1/'K values'!F4)))*((Head!G4-Head!F4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I5" s="1">
-        <f>'K values'!H4*((Head!H4-Head!G4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H4)+(1/'K values'!G4)))*((Head!H4-Head!G4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J5" s="1">
-        <f>'K values'!I4*((Head!I4-Head!H4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I4)+(1/'K values'!H4)))*((Head!I4-Head!H4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K5" s="1">
-        <f>'K values'!J4*((Head!J4-Head!I4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J4)+(1/'K values'!I4)))*((Head!J4-Head!I4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L5" s="1">
-        <f>'K values'!K4*((Head!K4-Head!J4)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K4)+(1/'K values'!J4)))*((Head!K4-Head!J4)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M5" s="1">
-        <f>'K values'!L4*((Head!L4-Head!K4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L4)+(1/'K values'!K4)))*((Head!L4-Head!K4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N5" s="1">
-        <f>'K values'!M4*((Head!M4-Head!L4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M4)+(1/'K values'!L4)))*((Head!M4-Head!L4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O5" s="1">
-        <f>'K values'!N4*((Head!N4-Head!M4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N4)+(1/'K values'!M4)))*((Head!N4-Head!M4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P5" s="1">
-        <f>'K values'!O4*((Head!O4-Head!N4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O4)+(1/'K values'!N4)))*((Head!O4-Head!N4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q5" s="1">
-        <f>'K values'!P4*((Head!P4-Head!O4)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P4)+(1/'K values'!O4)))*((Head!P4-Head!O4)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R5" s="1">
-        <f>'K values'!Q4*((Head!Q4-Head!P4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q4)+(1/'K values'!P4)))*((Head!Q4-Head!P4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S5" s="1">
-        <f>'K values'!R4*((Head!R4-Head!Q4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R4)+(1/'K values'!Q4)))*((Head!R4-Head!Q4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T5" s="1">
-        <f>'K values'!S4*((Head!S4-Head!R4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S4)+(1/'K values'!R4)))*((Head!S4-Head!R4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U5" s="1">
-        <f>'K values'!T4*((Head!T4-Head!S4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T4)+(1/'K values'!S4)))*((Head!T4-Head!S4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V5" s="1">
-        <f>'K values'!U4*((Head!U4-Head!T4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U4)+(1/'K values'!T4)))*((Head!U4-Head!T4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W5" s="1">
-        <f>'K values'!V4*((Head!V4-Head!U4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V4)+(1/'K values'!U4)))*((Head!V4-Head!U4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X5" s="1">
-        <f>'K values'!W4*((Head!W4-Head!V4)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W4)+(1/'K values'!V4)))*((Head!W4-Head!V4)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y5" s="1">
-        <f>'K values'!X4*((Head!X4-Head!W4)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X4)+(1/'K values'!W4)))*((Head!X4-Head!W4)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z5" s="1">
-        <f>'K values'!Y4*((Head!Y4-Head!X4)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y4)+(1/'K values'!X4)))*((Head!Y4-Head!X4)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA5">
         <v>300</v>
@@ -24449,104 +24450,104 @@
         <v>400</v>
       </c>
       <c r="B6" s="1">
-        <f>-1*'K values'!A5*((Head!A5)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A5)+(1/'K values'!A5)))*((Head!A5-Head!A5)/100))</f>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <f>'K values'!B5*((Head!B5-Head!A5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B5)+(1/'K values'!A5)))*((Head!B5-Head!A5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D6" s="1">
-        <f>'K values'!C5*((Head!C5-Head!B5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C5)+(1/'K values'!B5)))*((Head!C5-Head!B5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E6" s="1">
-        <f>'K values'!D5*((Head!D5-Head!C5)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D5)+(1/'K values'!C5)))*((Head!D5-Head!C5)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F6" s="1">
-        <f>'K values'!E5*((Head!E5-Head!D5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E5)+(1/'K values'!D5)))*((Head!E5-Head!D5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G6" s="1">
-        <f>'K values'!F5*((Head!F5-Head!E5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F5)+(1/'K values'!E5)))*((Head!F5-Head!E5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H6" s="1">
-        <f>'K values'!G5*((Head!G5-Head!F5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G5)+(1/'K values'!F5)))*((Head!G5-Head!F5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I6" s="1">
-        <f>'K values'!H5*((Head!H5-Head!G5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H5)+(1/'K values'!G5)))*((Head!H5-Head!G5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J6" s="1">
-        <f>'K values'!I5*((Head!I5-Head!H5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I5)+(1/'K values'!H5)))*((Head!I5-Head!H5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K6" s="1">
-        <f>'K values'!J5*((Head!J5-Head!I5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J5)+(1/'K values'!I5)))*((Head!J5-Head!I5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L6" s="1">
-        <f>'K values'!K5*((Head!K5-Head!J5)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K5)+(1/'K values'!J5)))*((Head!K5-Head!J5)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M6" s="1">
-        <f>'K values'!L5*((Head!L5-Head!K5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L5)+(1/'K values'!K5)))*((Head!L5-Head!K5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N6" s="1">
-        <f>'K values'!M5*((Head!M5-Head!L5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M5)+(1/'K values'!L5)))*((Head!M5-Head!L5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O6" s="1">
-        <f>'K values'!N5*((Head!N5-Head!M5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N5)+(1/'K values'!M5)))*((Head!N5-Head!M5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P6" s="1">
-        <f>'K values'!O5*((Head!O5-Head!N5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O5)+(1/'K values'!N5)))*((Head!O5-Head!N5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q6" s="1">
-        <f>'K values'!P5*((Head!P5-Head!O5)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P5)+(1/'K values'!O5)))*((Head!P5-Head!O5)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R6" s="1">
-        <f>'K values'!Q5*((Head!Q5-Head!P5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q5)+(1/'K values'!P5)))*((Head!Q5-Head!P5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S6" s="1">
-        <f>'K values'!R5*((Head!R5-Head!Q5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R5)+(1/'K values'!Q5)))*((Head!R5-Head!Q5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T6" s="1">
-        <f>'K values'!S5*((Head!S5-Head!R5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S5)+(1/'K values'!R5)))*((Head!S5-Head!R5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U6" s="1">
-        <f>'K values'!T5*((Head!T5-Head!S5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T5)+(1/'K values'!S5)))*((Head!T5-Head!S5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V6" s="1">
-        <f>'K values'!U5*((Head!U5-Head!T5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U5)+(1/'K values'!T5)))*((Head!U5-Head!T5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W6" s="1">
-        <f>'K values'!V5*((Head!V5-Head!U5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V5)+(1/'K values'!U5)))*((Head!V5-Head!U5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X6" s="1">
-        <f>'K values'!W5*((Head!W5-Head!V5)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W5)+(1/'K values'!V5)))*((Head!W5-Head!V5)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y6" s="1">
-        <f>'K values'!X5*((Head!X5-Head!W5)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X5)+(1/'K values'!W5)))*((Head!X5-Head!W5)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z6" s="1">
-        <f>'K values'!Y5*((Head!Y5-Head!X5)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y5)+(1/'K values'!X5)))*((Head!Y5-Head!X5)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA6">
         <v>400</v>
@@ -24557,104 +24558,104 @@
         <v>500</v>
       </c>
       <c r="B7" s="1">
-        <f>-1*'K values'!A6*((Head!A6)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A6)+(1/'K values'!A6)))*((Head!A6-Head!A6)/100))</f>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f>'K values'!B6*((Head!B6-Head!A6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B6)+(1/'K values'!A6)))*((Head!B6-Head!A6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D7" s="1">
-        <f>'K values'!C6*((Head!C6-Head!B6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C6)+(1/'K values'!B6)))*((Head!C6-Head!B6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E7" s="1">
-        <f>'K values'!D6*((Head!D6-Head!C6)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D6)+(1/'K values'!C6)))*((Head!D6-Head!C6)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F7" s="1">
-        <f>'K values'!E6*((Head!E6-Head!D6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E6)+(1/'K values'!D6)))*((Head!E6-Head!D6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G7" s="1">
-        <f>'K values'!F6*((Head!F6-Head!E6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F6)+(1/'K values'!E6)))*((Head!F6-Head!E6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H7" s="1">
-        <f>'K values'!G6*((Head!G6-Head!F6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G6)+(1/'K values'!F6)))*((Head!G6-Head!F6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I7" s="1">
-        <f>'K values'!H6*((Head!H6-Head!G6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H6)+(1/'K values'!G6)))*((Head!H6-Head!G6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J7" s="1">
-        <f>'K values'!I6*((Head!I6-Head!H6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I6)+(1/'K values'!H6)))*((Head!I6-Head!H6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K7" s="1">
-        <f>'K values'!J6*((Head!J6-Head!I6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J6)+(1/'K values'!I6)))*((Head!J6-Head!I6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L7" s="1">
-        <f>'K values'!K6*((Head!K6-Head!J6)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K6)+(1/'K values'!J6)))*((Head!K6-Head!J6)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M7" s="1">
-        <f>'K values'!L6*((Head!L6-Head!K6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L6)+(1/'K values'!K6)))*((Head!L6-Head!K6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N7" s="1">
-        <f>'K values'!M6*((Head!M6-Head!L6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M6)+(1/'K values'!L6)))*((Head!M6-Head!L6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O7" s="1">
-        <f>'K values'!N6*((Head!N6-Head!M6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N6)+(1/'K values'!M6)))*((Head!N6-Head!M6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P7" s="1">
-        <f>'K values'!O6*((Head!O6-Head!N6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O6)+(1/'K values'!N6)))*((Head!O6-Head!N6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q7" s="1">
-        <f>'K values'!P6*((Head!P6-Head!O6)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P6)+(1/'K values'!O6)))*((Head!P6-Head!O6)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R7" s="1">
-        <f>'K values'!Q6*((Head!Q6-Head!P6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q6)+(1/'K values'!P6)))*((Head!Q6-Head!P6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S7" s="1">
-        <f>'K values'!R6*((Head!R6-Head!Q6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R6)+(1/'K values'!Q6)))*((Head!R6-Head!Q6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T7" s="1">
-        <f>'K values'!S6*((Head!S6-Head!R6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S6)+(1/'K values'!R6)))*((Head!S6-Head!R6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U7" s="1">
-        <f>'K values'!T6*((Head!T6-Head!S6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T6)+(1/'K values'!S6)))*((Head!T6-Head!S6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V7" s="1">
-        <f>'K values'!U6*((Head!U6-Head!T6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U6)+(1/'K values'!T6)))*((Head!U6-Head!T6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W7" s="1">
-        <f>'K values'!V6*((Head!V6-Head!U6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V6)+(1/'K values'!U6)))*((Head!V6-Head!U6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X7" s="1">
-        <f>'K values'!W6*((Head!W6-Head!V6)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W6)+(1/'K values'!V6)))*((Head!W6-Head!V6)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y7" s="1">
-        <f>'K values'!X6*((Head!X6-Head!W6)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X6)+(1/'K values'!W6)))*((Head!X6-Head!W6)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z7" s="1">
-        <f>'K values'!Y6*((Head!Y6-Head!X6)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y6)+(1/'K values'!X6)))*((Head!Y6-Head!X6)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA7">
         <v>500</v>
@@ -24665,104 +24666,104 @@
         <v>600</v>
       </c>
       <c r="B8" s="1">
-        <f>-1*'K values'!A7*((Head!A7)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A7)+(1/'K values'!A7)))*((Head!A7-Head!A7)/100))</f>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <f>'K values'!B7*((Head!B7-Head!A7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B7)+(1/'K values'!A7)))*((Head!B7-Head!A7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D8" s="1">
-        <f>'K values'!C7*((Head!C7-Head!B7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C7)+(1/'K values'!B7)))*((Head!C7-Head!B7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E8" s="1">
-        <f>'K values'!D7*((Head!D7-Head!C7)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D7)+(1/'K values'!C7)))*((Head!D7-Head!C7)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F8" s="1">
-        <f>'K values'!E7*((Head!E7-Head!D7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E7)+(1/'K values'!D7)))*((Head!E7-Head!D7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G8" s="1">
-        <f>'K values'!F7*((Head!F7-Head!E7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F7)+(1/'K values'!E7)))*((Head!F7-Head!E7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H8" s="1">
-        <f>'K values'!G7*((Head!G7-Head!F7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G7)+(1/'K values'!F7)))*((Head!G7-Head!F7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I8" s="1">
-        <f>'K values'!H7*((Head!H7-Head!G7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H7)+(1/'K values'!G7)))*((Head!H7-Head!G7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J8" s="1">
-        <f>'K values'!I7*((Head!I7-Head!H7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I7)+(1/'K values'!H7)))*((Head!I7-Head!H7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K8" s="1">
-        <f>'K values'!J7*((Head!J7-Head!I7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J7)+(1/'K values'!I7)))*((Head!J7-Head!I7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L8" s="1">
-        <f>'K values'!K7*((Head!K7-Head!J7)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K7)+(1/'K values'!J7)))*((Head!K7-Head!J7)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M8" s="1">
-        <f>'K values'!L7*((Head!L7-Head!K7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L7)+(1/'K values'!K7)))*((Head!L7-Head!K7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N8" s="1">
-        <f>'K values'!M7*((Head!M7-Head!L7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M7)+(1/'K values'!L7)))*((Head!M7-Head!L7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O8" s="1">
-        <f>'K values'!N7*((Head!N7-Head!M7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N7)+(1/'K values'!M7)))*((Head!N7-Head!M7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P8" s="1">
-        <f>'K values'!O7*((Head!O7-Head!N7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O7)+(1/'K values'!N7)))*((Head!O7-Head!N7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q8" s="1">
-        <f>'K values'!P7*((Head!P7-Head!O7)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P7)+(1/'K values'!O7)))*((Head!P7-Head!O7)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R8" s="1">
-        <f>'K values'!Q7*((Head!Q7-Head!P7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q7)+(1/'K values'!P7)))*((Head!Q7-Head!P7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S8" s="1">
-        <f>'K values'!R7*((Head!R7-Head!Q7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R7)+(1/'K values'!Q7)))*((Head!R7-Head!Q7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T8" s="1">
-        <f>'K values'!S7*((Head!S7-Head!R7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S7)+(1/'K values'!R7)))*((Head!S7-Head!R7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U8" s="1">
-        <f>'K values'!T7*((Head!T7-Head!S7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T7)+(1/'K values'!S7)))*((Head!T7-Head!S7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V8" s="1">
-        <f>'K values'!U7*((Head!U7-Head!T7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U7)+(1/'K values'!T7)))*((Head!U7-Head!T7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W8" s="1">
-        <f>'K values'!V7*((Head!V7-Head!U7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V7)+(1/'K values'!U7)))*((Head!V7-Head!U7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X8" s="1">
-        <f>'K values'!W7*((Head!W7-Head!V7)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W7)+(1/'K values'!V7)))*((Head!W7-Head!V7)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y8" s="1">
-        <f>'K values'!X7*((Head!X7-Head!W7)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X7)+(1/'K values'!W7)))*((Head!X7-Head!W7)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z8" s="1">
-        <f>'K values'!Y7*((Head!Y7-Head!X7)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y7)+(1/'K values'!X7)))*((Head!Y7-Head!X7)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA8">
         <v>600</v>
@@ -24773,104 +24774,104 @@
         <v>700</v>
       </c>
       <c r="B9" s="1">
-        <f>-1*'K values'!A8*((Head!A8)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A8)+(1/'K values'!A8)))*((Head!A8-Head!A8)/100))</f>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <f>'K values'!B8*((Head!B8-Head!A8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B8)+(1/'K values'!A8)))*((Head!B8-Head!A8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D9" s="1">
-        <f>'K values'!C8*((Head!C8-Head!B8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C8)+(1/'K values'!B8)))*((Head!C8-Head!B8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E9" s="1">
-        <f>'K values'!D8*((Head!D8-Head!C8)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D8)+(1/'K values'!C8)))*((Head!D8-Head!C8)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F9" s="1">
-        <f>'K values'!E8*((Head!E8-Head!D8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E8)+(1/'K values'!D8)))*((Head!E8-Head!D8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G9" s="1">
-        <f>'K values'!F8*((Head!F8-Head!E8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F8)+(1/'K values'!E8)))*((Head!F8-Head!E8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H9" s="1">
-        <f>'K values'!G8*((Head!G8-Head!F8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G8)+(1/'K values'!F8)))*((Head!G8-Head!F8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I9" s="1">
-        <f>'K values'!H8*((Head!H8-Head!G8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H8)+(1/'K values'!G8)))*((Head!H8-Head!G8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J9" s="1">
-        <f>'K values'!I8*((Head!I8-Head!H8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I8)+(1/'K values'!H8)))*((Head!I8-Head!H8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K9" s="1">
-        <f>'K values'!J8*((Head!J8-Head!I8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J8)+(1/'K values'!I8)))*((Head!J8-Head!I8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L9" s="1">
-        <f>'K values'!K8*((Head!K8-Head!J8)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K8)+(1/'K values'!J8)))*((Head!K8-Head!J8)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M9" s="1">
-        <f>'K values'!L8*((Head!L8-Head!K8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L8)+(1/'K values'!K8)))*((Head!L8-Head!K8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N9" s="1">
-        <f>'K values'!M8*((Head!M8-Head!L8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M8)+(1/'K values'!L8)))*((Head!M8-Head!L8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O9" s="1">
-        <f>'K values'!N8*((Head!N8-Head!M8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N8)+(1/'K values'!M8)))*((Head!N8-Head!M8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P9" s="1">
-        <f>'K values'!O8*((Head!O8-Head!N8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O8)+(1/'K values'!N8)))*((Head!O8-Head!N8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q9" s="1">
-        <f>'K values'!P8*((Head!P8-Head!O8)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P8)+(1/'K values'!O8)))*((Head!P8-Head!O8)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R9" s="1">
-        <f>'K values'!Q8*((Head!Q8-Head!P8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q8)+(1/'K values'!P8)))*((Head!Q8-Head!P8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S9" s="1">
-        <f>'K values'!R8*((Head!R8-Head!Q8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R8)+(1/'K values'!Q8)))*((Head!R8-Head!Q8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T9" s="1">
-        <f>'K values'!S8*((Head!S8-Head!R8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S8)+(1/'K values'!R8)))*((Head!S8-Head!R8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U9" s="1">
-        <f>'K values'!T8*((Head!T8-Head!S8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T8)+(1/'K values'!S8)))*((Head!T8-Head!S8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V9" s="1">
-        <f>'K values'!U8*((Head!U8-Head!T8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U8)+(1/'K values'!T8)))*((Head!U8-Head!T8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W9" s="1">
-        <f>'K values'!V8*((Head!V8-Head!U8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V8)+(1/'K values'!U8)))*((Head!V8-Head!U8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X9" s="1">
-        <f>'K values'!W8*((Head!W8-Head!V8)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W8)+(1/'K values'!V8)))*((Head!W8-Head!V8)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y9" s="1">
-        <f>'K values'!X8*((Head!X8-Head!W8)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X8)+(1/'K values'!W8)))*((Head!X8-Head!W8)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z9" s="1">
-        <f>'K values'!Y8*((Head!Y8-Head!X8)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y8)+(1/'K values'!X8)))*((Head!Y8-Head!X8)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA9">
         <v>700</v>
@@ -24881,104 +24882,104 @@
         <v>800</v>
       </c>
       <c r="B10" s="1">
-        <f>-1*'K values'!A9*((Head!A9)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A9)+(1/'K values'!A9)))*((Head!A9-Head!A9)/100))</f>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
-        <f>'K values'!B9*((Head!B9-Head!A9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B9)+(1/'K values'!A9)))*((Head!B9-Head!A9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D10" s="1">
-        <f>'K values'!C9*((Head!C9-Head!B9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C9)+(1/'K values'!B9)))*((Head!C9-Head!B9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E10" s="1">
-        <f>'K values'!D9*((Head!D9-Head!C9)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D9)+(1/'K values'!C9)))*((Head!D9-Head!C9)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F10" s="1">
-        <f>'K values'!E9*((Head!E9-Head!D9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E9)+(1/'K values'!D9)))*((Head!E9-Head!D9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G10" s="1">
-        <f>'K values'!F9*((Head!F9-Head!E9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F9)+(1/'K values'!E9)))*((Head!F9-Head!E9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H10" s="1">
-        <f>'K values'!G9*((Head!G9-Head!F9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G9)+(1/'K values'!F9)))*((Head!G9-Head!F9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I10" s="1">
-        <f>'K values'!H9*((Head!H9-Head!G9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H9)+(1/'K values'!G9)))*((Head!H9-Head!G9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J10" s="1">
-        <f>'K values'!I9*((Head!I9-Head!H9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I9)+(1/'K values'!H9)))*((Head!I9-Head!H9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K10" s="1">
-        <f>'K values'!J9*((Head!J9-Head!I9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J9)+(1/'K values'!I9)))*((Head!J9-Head!I9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L10" s="1">
-        <f>'K values'!K9*((Head!K9-Head!J9)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K9)+(1/'K values'!J9)))*((Head!K9-Head!J9)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M10" s="1">
-        <f>'K values'!L9*((Head!L9-Head!K9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L9)+(1/'K values'!K9)))*((Head!L9-Head!K9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N10" s="1">
-        <f>'K values'!M9*((Head!M9-Head!L9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M9)+(1/'K values'!L9)))*((Head!M9-Head!L9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O10" s="1">
-        <f>'K values'!N9*((Head!N9-Head!M9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N9)+(1/'K values'!M9)))*((Head!N9-Head!M9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P10" s="1">
-        <f>'K values'!O9*((Head!O9-Head!N9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O9)+(1/'K values'!N9)))*((Head!O9-Head!N9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q10" s="1">
-        <f>'K values'!P9*((Head!P9-Head!O9)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P9)+(1/'K values'!O9)))*((Head!P9-Head!O9)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R10" s="1">
-        <f>'K values'!Q9*((Head!Q9-Head!P9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q9)+(1/'K values'!P9)))*((Head!Q9-Head!P9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S10" s="1">
-        <f>'K values'!R9*((Head!R9-Head!Q9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R9)+(1/'K values'!Q9)))*((Head!R9-Head!Q9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T10" s="1">
-        <f>'K values'!S9*((Head!S9-Head!R9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S9)+(1/'K values'!R9)))*((Head!S9-Head!R9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U10" s="1">
-        <f>'K values'!T9*((Head!T9-Head!S9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T9)+(1/'K values'!S9)))*((Head!T9-Head!S9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V10" s="1">
-        <f>'K values'!U9*((Head!U9-Head!T9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U9)+(1/'K values'!T9)))*((Head!U9-Head!T9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W10" s="1">
-        <f>'K values'!V9*((Head!V9-Head!U9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V9)+(1/'K values'!U9)))*((Head!V9-Head!U9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X10" s="1">
-        <f>'K values'!W9*((Head!W9-Head!V9)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W9)+(1/'K values'!V9)))*((Head!W9-Head!V9)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y10" s="1">
-        <f>'K values'!X9*((Head!X9-Head!W9)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X9)+(1/'K values'!W9)))*((Head!X9-Head!W9)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z10" s="1">
-        <f>'K values'!Y9*((Head!Y9-Head!X9)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y9)+(1/'K values'!X9)))*((Head!Y9-Head!X9)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA10">
         <v>800</v>
@@ -24989,104 +24990,104 @@
         <v>900</v>
       </c>
       <c r="B11" s="1">
-        <f>-1*'K values'!A10*((Head!A10)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A10)+(1/'K values'!A10)))*((Head!A10-Head!A10)/100))</f>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
-        <f>'K values'!B10*((Head!B10-Head!A10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B10)+(1/'K values'!A10)))*((Head!B10-Head!A10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D11" s="1">
-        <f>'K values'!C10*((Head!C10-Head!B10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C10)+(1/'K values'!B10)))*((Head!C10-Head!B10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E11" s="1">
-        <f>'K values'!D10*((Head!D10-Head!C10)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D10)+(1/'K values'!C10)))*((Head!D10-Head!C10)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F11" s="1">
-        <f>'K values'!E10*((Head!E10-Head!D10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E10)+(1/'K values'!D10)))*((Head!E10-Head!D10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G11" s="1">
-        <f>'K values'!F10*((Head!F10-Head!E10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F10)+(1/'K values'!E10)))*((Head!F10-Head!E10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H11" s="1">
-        <f>'K values'!G10*((Head!G10-Head!F10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G10)+(1/'K values'!F10)))*((Head!G10-Head!F10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I11" s="1">
-        <f>'K values'!H10*((Head!H10-Head!G10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H10)+(1/'K values'!G10)))*((Head!H10-Head!G10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J11" s="1">
-        <f>'K values'!I10*((Head!I10-Head!H10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I10)+(1/'K values'!H10)))*((Head!I10-Head!H10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K11" s="1">
-        <f>'K values'!J10*((Head!J10-Head!I10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J10)+(1/'K values'!I10)))*((Head!J10-Head!I10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L11" s="1">
-        <f>'K values'!K10*((Head!K10-Head!J10)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K10)+(1/'K values'!J10)))*((Head!K10-Head!J10)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M11" s="1">
-        <f>'K values'!L10*((Head!L10-Head!K10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L10)+(1/'K values'!K10)))*((Head!L10-Head!K10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N11" s="1">
-        <f>'K values'!M10*((Head!M10-Head!L10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M10)+(1/'K values'!L10)))*((Head!M10-Head!L10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O11" s="1">
-        <f>'K values'!N10*((Head!N10-Head!M10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N10)+(1/'K values'!M10)))*((Head!N10-Head!M10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P11" s="1">
-        <f>'K values'!O10*((Head!O10-Head!N10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O10)+(1/'K values'!N10)))*((Head!O10-Head!N10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q11" s="1">
-        <f>'K values'!P10*((Head!P10-Head!O10)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P10)+(1/'K values'!O10)))*((Head!P10-Head!O10)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R11" s="1">
-        <f>'K values'!Q10*((Head!Q10-Head!P10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q10)+(1/'K values'!P10)))*((Head!Q10-Head!P10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S11" s="1">
-        <f>'K values'!R10*((Head!R10-Head!Q10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R10)+(1/'K values'!Q10)))*((Head!R10-Head!Q10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T11" s="1">
-        <f>'K values'!S10*((Head!S10-Head!R10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S10)+(1/'K values'!R10)))*((Head!S10-Head!R10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U11" s="1">
-        <f>'K values'!T10*((Head!T10-Head!S10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T10)+(1/'K values'!S10)))*((Head!T10-Head!S10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V11" s="1">
-        <f>'K values'!U10*((Head!U10-Head!T10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U10)+(1/'K values'!T10)))*((Head!U10-Head!T10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W11" s="1">
-        <f>'K values'!V10*((Head!V10-Head!U10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V10)+(1/'K values'!U10)))*((Head!V10-Head!U10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X11" s="1">
-        <f>'K values'!W10*((Head!W10-Head!V10)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W10)+(1/'K values'!V10)))*((Head!W10-Head!V10)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y11" s="1">
-        <f>'K values'!X10*((Head!X10-Head!W10)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X10)+(1/'K values'!W10)))*((Head!X10-Head!W10)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z11" s="1">
-        <f>'K values'!Y10*((Head!Y10-Head!X10)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y10)+(1/'K values'!X10)))*((Head!Y10-Head!X10)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA11">
         <v>900</v>
@@ -25097,104 +25098,104 @@
         <v>1000</v>
       </c>
       <c r="B12" s="1">
-        <f>-1*'K values'!A11*((Head!A11)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A11)+(1/'K values'!A11)))*((Head!A11-Head!A11)/100))</f>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <f>'K values'!B11*((Head!B11-Head!A11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B11)+(1/'K values'!A11)))*((Head!B11-Head!A11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D12" s="1">
-        <f>'K values'!C11*((Head!C11-Head!B11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C11)+(1/'K values'!B11)))*((Head!C11-Head!B11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E12" s="1">
-        <f>'K values'!D11*((Head!D11-Head!C11)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D11)+(1/'K values'!C11)))*((Head!D11-Head!C11)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F12" s="1">
-        <f>'K values'!E11*((Head!E11-Head!D11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E11)+(1/'K values'!D11)))*((Head!E11-Head!D11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G12" s="1">
-        <f>'K values'!F11*((Head!F11-Head!E11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F11)+(1/'K values'!E11)))*((Head!F11-Head!E11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H12" s="1">
-        <f>'K values'!G11*((Head!G11-Head!F11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G11)+(1/'K values'!F11)))*((Head!G11-Head!F11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I12" s="1">
-        <f>'K values'!H11*((Head!H11-Head!G11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H11)+(1/'K values'!G11)))*((Head!H11-Head!G11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J12" s="1">
-        <f>'K values'!I11*((Head!I11-Head!H11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I11)+(1/'K values'!H11)))*((Head!I11-Head!H11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K12" s="1">
-        <f>'K values'!J11*((Head!J11-Head!I11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J11)+(1/'K values'!I11)))*((Head!J11-Head!I11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L12" s="1">
-        <f>'K values'!K11*((Head!K11-Head!J11)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K11)+(1/'K values'!J11)))*((Head!K11-Head!J11)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M12" s="1">
-        <f>'K values'!L11*((Head!L11-Head!K11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L11)+(1/'K values'!K11)))*((Head!L11-Head!K11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N12" s="1">
-        <f>'K values'!M11*((Head!M11-Head!L11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M11)+(1/'K values'!L11)))*((Head!M11-Head!L11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O12" s="1">
-        <f>'K values'!N11*((Head!N11-Head!M11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N11)+(1/'K values'!M11)))*((Head!N11-Head!M11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P12" s="1">
-        <f>'K values'!O11*((Head!O11-Head!N11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O11)+(1/'K values'!N11)))*((Head!O11-Head!N11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q12" s="1">
-        <f>'K values'!P11*((Head!P11-Head!O11)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P11)+(1/'K values'!O11)))*((Head!P11-Head!O11)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R12" s="1">
-        <f>'K values'!Q11*((Head!Q11-Head!P11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q11)+(1/'K values'!P11)))*((Head!Q11-Head!P11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S12" s="1">
-        <f>'K values'!R11*((Head!R11-Head!Q11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R11)+(1/'K values'!Q11)))*((Head!R11-Head!Q11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T12" s="1">
-        <f>'K values'!S11*((Head!S11-Head!R11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S11)+(1/'K values'!R11)))*((Head!S11-Head!R11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U12" s="1">
-        <f>'K values'!T11*((Head!T11-Head!S11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T11)+(1/'K values'!S11)))*((Head!T11-Head!S11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V12" s="1">
-        <f>'K values'!U11*((Head!U11-Head!T11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U11)+(1/'K values'!T11)))*((Head!U11-Head!T11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W12" s="1">
-        <f>'K values'!V11*((Head!V11-Head!U11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V11)+(1/'K values'!U11)))*((Head!V11-Head!U11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X12" s="1">
-        <f>'K values'!W11*((Head!W11-Head!V11)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W11)+(1/'K values'!V11)))*((Head!W11-Head!V11)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y12" s="1">
-        <f>'K values'!X11*((Head!X11-Head!W11)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X11)+(1/'K values'!W11)))*((Head!X11-Head!W11)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z12" s="1">
-        <f>'K values'!Y11*((Head!Y11-Head!X11)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y11)+(1/'K values'!X11)))*((Head!Y11-Head!X11)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA12">
         <v>1000</v>
@@ -25205,104 +25206,104 @@
         <v>1100</v>
       </c>
       <c r="B13" s="1">
-        <f>-1*'K values'!A12*((Head!A12)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A12)+(1/'K values'!A12)))*((Head!A12-Head!A12)/100))</f>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <f>'K values'!B12*((Head!B12-Head!A12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B12)+(1/'K values'!A12)))*((Head!B12-Head!A12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D13" s="1">
-        <f>'K values'!C12*((Head!C12-Head!B12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C12)+(1/'K values'!B12)))*((Head!C12-Head!B12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E13" s="1">
-        <f>'K values'!D12*((Head!D12-Head!C12)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D12)+(1/'K values'!C12)))*((Head!D12-Head!C12)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F13" s="1">
-        <f>'K values'!E12*((Head!E12-Head!D12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E12)+(1/'K values'!D12)))*((Head!E12-Head!D12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G13" s="1">
-        <f>'K values'!F12*((Head!F12-Head!E12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F12)+(1/'K values'!E12)))*((Head!F12-Head!E12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H13" s="1">
-        <f>'K values'!G12*((Head!G12-Head!F12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G12)+(1/'K values'!F12)))*((Head!G12-Head!F12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I13" s="1">
-        <f>'K values'!H12*((Head!H12-Head!G12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H12)+(1/'K values'!G12)))*((Head!H12-Head!G12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J13" s="1">
-        <f>'K values'!I12*((Head!I12-Head!H12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I12)+(1/'K values'!H12)))*((Head!I12-Head!H12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K13" s="1">
-        <f>'K values'!J12*((Head!J12-Head!I12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J12)+(1/'K values'!I12)))*((Head!J12-Head!I12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L13" s="1">
-        <f>'K values'!K12*((Head!K12-Head!J12)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K12)+(1/'K values'!J12)))*((Head!K12-Head!J12)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M13" s="1">
-        <f>'K values'!L12*((Head!L12-Head!K12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L12)+(1/'K values'!K12)))*((Head!L12-Head!K12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N13" s="1">
-        <f>'K values'!M12*((Head!M12-Head!L12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M12)+(1/'K values'!L12)))*((Head!M12-Head!L12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O13" s="1">
-        <f>'K values'!N12*((Head!N12-Head!M12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N12)+(1/'K values'!M12)))*((Head!N12-Head!M12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P13" s="1">
-        <f>'K values'!O12*((Head!O12-Head!N12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O12)+(1/'K values'!N12)))*((Head!O12-Head!N12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q13" s="1">
-        <f>'K values'!P12*((Head!P12-Head!O12)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P12)+(1/'K values'!O12)))*((Head!P12-Head!O12)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R13" s="1">
-        <f>'K values'!Q12*((Head!Q12-Head!P12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q12)+(1/'K values'!P12)))*((Head!Q12-Head!P12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S13" s="1">
-        <f>'K values'!R12*((Head!R12-Head!Q12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R12)+(1/'K values'!Q12)))*((Head!R12-Head!Q12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T13" s="1">
-        <f>'K values'!S12*((Head!S12-Head!R12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S12)+(1/'K values'!R12)))*((Head!S12-Head!R12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U13" s="1">
-        <f>'K values'!T12*((Head!T12-Head!S12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T12)+(1/'K values'!S12)))*((Head!T12-Head!S12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V13" s="1">
-        <f>'K values'!U12*((Head!U12-Head!T12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U12)+(1/'K values'!T12)))*((Head!U12-Head!T12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W13" s="1">
-        <f>'K values'!V12*((Head!V12-Head!U12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V12)+(1/'K values'!U12)))*((Head!V12-Head!U12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X13" s="1">
-        <f>'K values'!W12*((Head!W12-Head!V12)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W12)+(1/'K values'!V12)))*((Head!W12-Head!V12)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y13" s="1">
-        <f>'K values'!X12*((Head!X12-Head!W12)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X12)+(1/'K values'!W12)))*((Head!X12-Head!W12)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z13" s="1">
-        <f>'K values'!Y12*((Head!Y12-Head!X12)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y12)+(1/'K values'!X12)))*((Head!Y12-Head!X12)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA13">
         <v>1100</v>
@@ -25313,104 +25314,104 @@
         <v>1200</v>
       </c>
       <c r="B14" s="1">
-        <f>-1*'K values'!A13*((Head!A13)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A13)+(1/'K values'!A13)))*((Head!A13-Head!A13)/100))</f>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <f>'K values'!B13*((Head!B13-Head!A13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B13)+(1/'K values'!A13)))*((Head!B13-Head!A13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D14" s="1">
-        <f>'K values'!C13*((Head!C13-Head!B13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C13)+(1/'K values'!B13)))*((Head!C13-Head!B13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E14" s="1">
-        <f>'K values'!D13*((Head!D13-Head!C13)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D13)+(1/'K values'!C13)))*((Head!D13-Head!C13)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F14" s="1">
-        <f>'K values'!E13*((Head!E13-Head!D13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E13)+(1/'K values'!D13)))*((Head!E13-Head!D13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G14" s="1">
-        <f>'K values'!F13*((Head!F13-Head!E13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F13)+(1/'K values'!E13)))*((Head!F13-Head!E13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H14" s="1">
-        <f>'K values'!G13*((Head!G13-Head!F13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G13)+(1/'K values'!F13)))*((Head!G13-Head!F13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I14" s="1">
-        <f>'K values'!H13*((Head!H13-Head!G13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H13)+(1/'K values'!G13)))*((Head!H13-Head!G13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J14" s="1">
-        <f>'K values'!I13*((Head!I13-Head!H13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I13)+(1/'K values'!H13)))*((Head!I13-Head!H13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K14" s="1">
-        <f>'K values'!J13*((Head!J13-Head!I13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J13)+(1/'K values'!I13)))*((Head!J13-Head!I13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L14" s="1">
-        <f>'K values'!K13*((Head!K13-Head!J13)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K13)+(1/'K values'!J13)))*((Head!K13-Head!J13)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M14" s="1">
-        <f>'K values'!L13*((Head!L13-Head!K13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L13)+(1/'K values'!K13)))*((Head!L13-Head!K13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N14" s="1">
-        <f>'K values'!M13*((Head!M13-Head!L13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M13)+(1/'K values'!L13)))*((Head!M13-Head!L13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O14" s="1">
-        <f>'K values'!N13*((Head!N13-Head!M13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N13)+(1/'K values'!M13)))*((Head!N13-Head!M13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P14" s="1">
-        <f>'K values'!O13*((Head!O13-Head!N13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O13)+(1/'K values'!N13)))*((Head!O13-Head!N13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q14" s="1">
-        <f>'K values'!P13*((Head!P13-Head!O13)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P13)+(1/'K values'!O13)))*((Head!P13-Head!O13)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R14" s="1">
-        <f>'K values'!Q13*((Head!Q13-Head!P13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q13)+(1/'K values'!P13)))*((Head!Q13-Head!P13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S14" s="1">
-        <f>'K values'!R13*((Head!R13-Head!Q13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R13)+(1/'K values'!Q13)))*((Head!R13-Head!Q13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T14" s="1">
-        <f>'K values'!S13*((Head!S13-Head!R13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S13)+(1/'K values'!R13)))*((Head!S13-Head!R13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U14" s="1">
-        <f>'K values'!T13*((Head!T13-Head!S13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T13)+(1/'K values'!S13)))*((Head!T13-Head!S13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V14" s="1">
-        <f>'K values'!U13*((Head!U13-Head!T13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U13)+(1/'K values'!T13)))*((Head!U13-Head!T13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W14" s="1">
-        <f>'K values'!V13*((Head!V13-Head!U13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V13)+(1/'K values'!U13)))*((Head!V13-Head!U13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X14" s="1">
-        <f>'K values'!W13*((Head!W13-Head!V13)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W13)+(1/'K values'!V13)))*((Head!W13-Head!V13)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y14" s="1">
-        <f>'K values'!X13*((Head!X13-Head!W13)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X13)+(1/'K values'!W13)))*((Head!X13-Head!W13)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z14" s="1">
-        <f>'K values'!Y13*((Head!Y13-Head!X13)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y13)+(1/'K values'!X13)))*((Head!Y13-Head!X13)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA14">
         <v>1200</v>
@@ -25421,104 +25422,104 @@
         <v>1300</v>
       </c>
       <c r="B15" s="1">
-        <f>-1*'K values'!A14*((Head!A14)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A14)+(1/'K values'!A14)))*((Head!A14-Head!A14)/100))</f>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <f>'K values'!B14*((Head!B14-Head!A14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B14)+(1/'K values'!A14)))*((Head!B14-Head!A14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D15" s="1">
-        <f>'K values'!C14*((Head!C14-Head!B14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C14)+(1/'K values'!B14)))*((Head!C14-Head!B14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E15" s="1">
-        <f>'K values'!D14*((Head!D14-Head!C14)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D14)+(1/'K values'!C14)))*((Head!D14-Head!C14)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F15" s="1">
-        <f>'K values'!E14*((Head!E14-Head!D14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E14)+(1/'K values'!D14)))*((Head!E14-Head!D14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G15" s="1">
-        <f>'K values'!F14*((Head!F14-Head!E14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F14)+(1/'K values'!E14)))*((Head!F14-Head!E14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H15" s="1">
-        <f>'K values'!G14*((Head!G14-Head!F14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G14)+(1/'K values'!F14)))*((Head!G14-Head!F14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I15" s="1">
-        <f>'K values'!H14*((Head!H14-Head!G14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H14)+(1/'K values'!G14)))*((Head!H14-Head!G14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J15" s="1">
-        <f>'K values'!I14*((Head!I14-Head!H14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I14)+(1/'K values'!H14)))*((Head!I14-Head!H14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K15" s="1">
-        <f>'K values'!J14*((Head!J14-Head!I14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J14)+(1/'K values'!I14)))*((Head!J14-Head!I14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L15" s="1">
-        <f>'K values'!K14*((Head!K14-Head!J14)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K14)+(1/'K values'!J14)))*((Head!K14-Head!J14)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M15" s="1">
-        <f>'K values'!L14*((Head!L14-Head!K14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L14)+(1/'K values'!K14)))*((Head!L14-Head!K14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N15" s="1">
-        <f>'K values'!M14*((Head!M14-Head!L14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M14)+(1/'K values'!L14)))*((Head!M14-Head!L14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O15" s="1">
-        <f>'K values'!N14*((Head!N14-Head!M14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N14)+(1/'K values'!M14)))*((Head!N14-Head!M14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P15" s="1">
-        <f>'K values'!O14*((Head!O14-Head!N14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O14)+(1/'K values'!N14)))*((Head!O14-Head!N14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q15" s="1">
-        <f>'K values'!P14*((Head!P14-Head!O14)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P14)+(1/'K values'!O14)))*((Head!P14-Head!O14)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R15" s="1">
-        <f>'K values'!Q14*((Head!Q14-Head!P14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q14)+(1/'K values'!P14)))*((Head!Q14-Head!P14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S15" s="1">
-        <f>'K values'!R14*((Head!R14-Head!Q14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R14)+(1/'K values'!Q14)))*((Head!R14-Head!Q14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T15" s="1">
-        <f>'K values'!S14*((Head!S14-Head!R14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S14)+(1/'K values'!R14)))*((Head!S14-Head!R14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U15" s="1">
-        <f>'K values'!T14*((Head!T14-Head!S14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T14)+(1/'K values'!S14)))*((Head!T14-Head!S14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V15" s="1">
-        <f>'K values'!U14*((Head!U14-Head!T14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U14)+(1/'K values'!T14)))*((Head!U14-Head!T14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W15" s="1">
-        <f>'K values'!V14*((Head!V14-Head!U14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V14)+(1/'K values'!U14)))*((Head!V14-Head!U14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X15" s="1">
-        <f>'K values'!W14*((Head!W14-Head!V14)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W14)+(1/'K values'!V14)))*((Head!W14-Head!V14)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y15" s="1">
-        <f>'K values'!X14*((Head!X14-Head!W14)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X14)+(1/'K values'!W14)))*((Head!X14-Head!W14)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z15" s="1">
-        <f>'K values'!Y14*((Head!Y14-Head!X14)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y14)+(1/'K values'!X14)))*((Head!Y14-Head!X14)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA15">
         <v>1300</v>
@@ -25529,104 +25530,104 @@
         <v>1400</v>
       </c>
       <c r="B16" s="1">
-        <f>-1*'K values'!A15*((Head!A15)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A15)+(1/'K values'!A15)))*((Head!A15-Head!A15)/100))</f>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
-        <f>'K values'!B15*((Head!B15-Head!A15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B15)+(1/'K values'!A15)))*((Head!B15-Head!A15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D16" s="1">
-        <f>'K values'!C15*((Head!C15-Head!B15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C15)+(1/'K values'!B15)))*((Head!C15-Head!B15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E16" s="1">
-        <f>'K values'!D15*((Head!D15-Head!C15)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D15)+(1/'K values'!C15)))*((Head!D15-Head!C15)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>'K values'!E15*((Head!E15-Head!D15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E15)+(1/'K values'!D15)))*((Head!E15-Head!D15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G16" s="1">
-        <f>'K values'!F15*((Head!F15-Head!E15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F15)+(1/'K values'!E15)))*((Head!F15-Head!E15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H16" s="1">
-        <f>'K values'!G15*((Head!G15-Head!F15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G15)+(1/'K values'!F15)))*((Head!G15-Head!F15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I16" s="1">
-        <f>'K values'!H15*((Head!H15-Head!G15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H15)+(1/'K values'!G15)))*((Head!H15-Head!G15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J16" s="1">
-        <f>'K values'!I15*((Head!I15-Head!H15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I15)+(1/'K values'!H15)))*((Head!I15-Head!H15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K16" s="1">
-        <f>'K values'!J15*((Head!J15-Head!I15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J15)+(1/'K values'!I15)))*((Head!J15-Head!I15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L16" s="1">
-        <f>'K values'!K15*((Head!K15-Head!J15)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K15)+(1/'K values'!J15)))*((Head!K15-Head!J15)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M16" s="1">
-        <f>'K values'!L15*((Head!L15-Head!K15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L15)+(1/'K values'!K15)))*((Head!L15-Head!K15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N16" s="1">
-        <f>'K values'!M15*((Head!M15-Head!L15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M15)+(1/'K values'!L15)))*((Head!M15-Head!L15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O16" s="1">
-        <f>'K values'!N15*((Head!N15-Head!M15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N15)+(1/'K values'!M15)))*((Head!N15-Head!M15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P16" s="1">
-        <f>'K values'!O15*((Head!O15-Head!N15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O15)+(1/'K values'!N15)))*((Head!O15-Head!N15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q16" s="1">
-        <f>'K values'!P15*((Head!P15-Head!O15)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P15)+(1/'K values'!O15)))*((Head!P15-Head!O15)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R16" s="1">
-        <f>'K values'!Q15*((Head!Q15-Head!P15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q15)+(1/'K values'!P15)))*((Head!Q15-Head!P15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S16" s="1">
-        <f>'K values'!R15*((Head!R15-Head!Q15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R15)+(1/'K values'!Q15)))*((Head!R15-Head!Q15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T16" s="1">
-        <f>'K values'!S15*((Head!S15-Head!R15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S15)+(1/'K values'!R15)))*((Head!S15-Head!R15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U16" s="1">
-        <f>'K values'!T15*((Head!T15-Head!S15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T15)+(1/'K values'!S15)))*((Head!T15-Head!S15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V16" s="1">
-        <f>'K values'!U15*((Head!U15-Head!T15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U15)+(1/'K values'!T15)))*((Head!U15-Head!T15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W16" s="1">
-        <f>'K values'!V15*((Head!V15-Head!U15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V15)+(1/'K values'!U15)))*((Head!V15-Head!U15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X16" s="1">
-        <f>'K values'!W15*((Head!W15-Head!V15)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W15)+(1/'K values'!V15)))*((Head!W15-Head!V15)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y16" s="1">
-        <f>'K values'!X15*((Head!X15-Head!W15)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X15)+(1/'K values'!W15)))*((Head!X15-Head!W15)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z16" s="1">
-        <f>'K values'!Y15*((Head!Y15-Head!X15)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y15)+(1/'K values'!X15)))*((Head!Y15-Head!X15)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA16">
         <v>1400</v>
@@ -25637,104 +25638,104 @@
         <v>1500</v>
       </c>
       <c r="B17" s="1">
-        <f>-1*'K values'!A16*((Head!A16)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A16)+(1/'K values'!A16)))*((Head!A16-Head!A16)/100))</f>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <f>'K values'!B16*((Head!B16-Head!A16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B16)+(1/'K values'!A16)))*((Head!B16-Head!A16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D17" s="1">
-        <f>'K values'!C16*((Head!C16-Head!B16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C16)+(1/'K values'!B16)))*((Head!C16-Head!B16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E17" s="1">
-        <f>'K values'!D16*((Head!D16-Head!C16)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D16)+(1/'K values'!C16)))*((Head!D16-Head!C16)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>'K values'!E16*((Head!E16-Head!D16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E16)+(1/'K values'!D16)))*((Head!E16-Head!D16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G17" s="1">
-        <f>'K values'!F16*((Head!F16-Head!E16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F16)+(1/'K values'!E16)))*((Head!F16-Head!E16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H17" s="1">
-        <f>'K values'!G16*((Head!G16-Head!F16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G16)+(1/'K values'!F16)))*((Head!G16-Head!F16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I17" s="1">
-        <f>'K values'!H16*((Head!H16-Head!G16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H16)+(1/'K values'!G16)))*((Head!H16-Head!G16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J17" s="1">
-        <f>'K values'!I16*((Head!I16-Head!H16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I16)+(1/'K values'!H16)))*((Head!I16-Head!H16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K17" s="1">
-        <f>'K values'!J16*((Head!J16-Head!I16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J16)+(1/'K values'!I16)))*((Head!J16-Head!I16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L17" s="1">
-        <f>'K values'!K16*((Head!K16-Head!J16)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K16)+(1/'K values'!J16)))*((Head!K16-Head!J16)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M17" s="1">
-        <f>'K values'!L16*((Head!L16-Head!K16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L16)+(1/'K values'!K16)))*((Head!L16-Head!K16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N17" s="1">
-        <f>'K values'!M16*((Head!M16-Head!L16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M16)+(1/'K values'!L16)))*((Head!M16-Head!L16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O17" s="1">
-        <f>'K values'!N16*((Head!N16-Head!M16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N16)+(1/'K values'!M16)))*((Head!N16-Head!M16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P17" s="1">
-        <f>'K values'!O16*((Head!O16-Head!N16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O16)+(1/'K values'!N16)))*((Head!O16-Head!N16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q17" s="1">
-        <f>'K values'!P16*((Head!P16-Head!O16)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P16)+(1/'K values'!O16)))*((Head!P16-Head!O16)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R17" s="1">
-        <f>'K values'!Q16*((Head!Q16-Head!P16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q16)+(1/'K values'!P16)))*((Head!Q16-Head!P16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S17" s="1">
-        <f>'K values'!R16*((Head!R16-Head!Q16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R16)+(1/'K values'!Q16)))*((Head!R16-Head!Q16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T17" s="1">
-        <f>'K values'!S16*((Head!S16-Head!R16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S16)+(1/'K values'!R16)))*((Head!S16-Head!R16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U17" s="1">
-        <f>'K values'!T16*((Head!T16-Head!S16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T16)+(1/'K values'!S16)))*((Head!T16-Head!S16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V17" s="1">
-        <f>'K values'!U16*((Head!U16-Head!T16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U16)+(1/'K values'!T16)))*((Head!U16-Head!T16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W17" s="1">
-        <f>'K values'!V16*((Head!V16-Head!U16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V16)+(1/'K values'!U16)))*((Head!V16-Head!U16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X17" s="1">
-        <f>'K values'!W16*((Head!W16-Head!V16)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W16)+(1/'K values'!V16)))*((Head!W16-Head!V16)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y17" s="1">
-        <f>'K values'!X16*((Head!X16-Head!W16)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X16)+(1/'K values'!W16)))*((Head!X16-Head!W16)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z17" s="1">
-        <f>'K values'!Y16*((Head!Y16-Head!X16)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y16)+(1/'K values'!X16)))*((Head!Y16-Head!X16)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA17">
         <v>1500</v>
@@ -25745,104 +25746,104 @@
         <v>1600</v>
       </c>
       <c r="B18" s="1">
-        <f>-1*'K values'!A17*((Head!A17)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A17)+(1/'K values'!A17)))*((Head!A17-Head!A17)/100))</f>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
-        <f>'K values'!B17*((Head!B17-Head!A17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B17)+(1/'K values'!A17)))*((Head!B17-Head!A17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D18" s="1">
-        <f>'K values'!C17*((Head!C17-Head!B17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C17)+(1/'K values'!B17)))*((Head!C17-Head!B17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E18" s="1">
-        <f>'K values'!D17*((Head!D17-Head!C17)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D17)+(1/'K values'!C17)))*((Head!D17-Head!C17)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>'K values'!E17*((Head!E17-Head!D17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E17)+(1/'K values'!D17)))*((Head!E17-Head!D17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G18" s="1">
-        <f>'K values'!F17*((Head!F17-Head!E17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F17)+(1/'K values'!E17)))*((Head!F17-Head!E17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H18" s="1">
-        <f>'K values'!G17*((Head!G17-Head!F17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G17)+(1/'K values'!F17)))*((Head!G17-Head!F17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I18" s="1">
-        <f>'K values'!H17*((Head!H17-Head!G17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H17)+(1/'K values'!G17)))*((Head!H17-Head!G17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J18" s="1">
-        <f>'K values'!I17*((Head!I17-Head!H17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I17)+(1/'K values'!H17)))*((Head!I17-Head!H17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K18" s="1">
-        <f>'K values'!J17*((Head!J17-Head!I17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J17)+(1/'K values'!I17)))*((Head!J17-Head!I17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L18" s="1">
-        <f>'K values'!K17*((Head!K17-Head!J17)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K17)+(1/'K values'!J17)))*((Head!K17-Head!J17)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M18" s="1">
-        <f>'K values'!L17*((Head!L17-Head!K17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L17)+(1/'K values'!K17)))*((Head!L17-Head!K17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N18" s="1">
-        <f>'K values'!M17*((Head!M17-Head!L17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M17)+(1/'K values'!L17)))*((Head!M17-Head!L17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O18" s="1">
-        <f>'K values'!N17*((Head!N17-Head!M17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N17)+(1/'K values'!M17)))*((Head!N17-Head!M17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P18" s="1">
-        <f>'K values'!O17*((Head!O17-Head!N17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O17)+(1/'K values'!N17)))*((Head!O17-Head!N17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q18" s="1">
-        <f>'K values'!P17*((Head!P17-Head!O17)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P17)+(1/'K values'!O17)))*((Head!P17-Head!O17)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R18" s="1">
-        <f>'K values'!Q17*((Head!Q17-Head!P17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q17)+(1/'K values'!P17)))*((Head!Q17-Head!P17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S18" s="1">
-        <f>'K values'!R17*((Head!R17-Head!Q17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R17)+(1/'K values'!Q17)))*((Head!R17-Head!Q17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T18" s="1">
-        <f>'K values'!S17*((Head!S17-Head!R17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S17)+(1/'K values'!R17)))*((Head!S17-Head!R17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U18" s="1">
-        <f>'K values'!T17*((Head!T17-Head!S17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T17)+(1/'K values'!S17)))*((Head!T17-Head!S17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V18" s="1">
-        <f>'K values'!U17*((Head!U17-Head!T17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U17)+(1/'K values'!T17)))*((Head!U17-Head!T17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W18" s="1">
-        <f>'K values'!V17*((Head!V17-Head!U17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V17)+(1/'K values'!U17)))*((Head!V17-Head!U17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X18" s="1">
-        <f>'K values'!W17*((Head!W17-Head!V17)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W17)+(1/'K values'!V17)))*((Head!W17-Head!V17)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y18" s="1">
-        <f>'K values'!X17*((Head!X17-Head!W17)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X17)+(1/'K values'!W17)))*((Head!X17-Head!W17)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z18" s="1">
-        <f>'K values'!Y17*((Head!Y17-Head!X17)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y17)+(1/'K values'!X17)))*((Head!Y17-Head!X17)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA18">
         <v>1600</v>
@@ -25853,104 +25854,104 @@
         <v>1700</v>
       </c>
       <c r="B19" s="1">
-        <f>-1*'K values'!A18*((Head!A18)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A18)+(1/'K values'!A18)))*((Head!A18-Head!A18)/100))</f>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>'K values'!B18*((Head!B18-Head!A18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B18)+(1/'K values'!A18)))*((Head!B18-Head!A18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D19" s="1">
-        <f>'K values'!C18*((Head!C18-Head!B18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C18)+(1/'K values'!B18)))*((Head!C18-Head!B18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E19" s="1">
-        <f>'K values'!D18*((Head!D18-Head!C18)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D18)+(1/'K values'!C18)))*((Head!D18-Head!C18)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>'K values'!E18*((Head!E18-Head!D18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E18)+(1/'K values'!D18)))*((Head!E18-Head!D18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G19" s="1">
-        <f>'K values'!F18*((Head!F18-Head!E18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F18)+(1/'K values'!E18)))*((Head!F18-Head!E18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H19" s="1">
-        <f>'K values'!G18*((Head!G18-Head!F18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G18)+(1/'K values'!F18)))*((Head!G18-Head!F18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I19" s="1">
-        <f>'K values'!H18*((Head!H18-Head!G18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H18)+(1/'K values'!G18)))*((Head!H18-Head!G18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J19" s="1">
-        <f>'K values'!I18*((Head!I18-Head!H18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I18)+(1/'K values'!H18)))*((Head!I18-Head!H18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K19" s="1">
-        <f>'K values'!J18*((Head!J18-Head!I18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J18)+(1/'K values'!I18)))*((Head!J18-Head!I18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L19" s="1">
-        <f>'K values'!K18*((Head!K18-Head!J18)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K18)+(1/'K values'!J18)))*((Head!K18-Head!J18)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M19" s="1">
-        <f>'K values'!L18*((Head!L18-Head!K18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L18)+(1/'K values'!K18)))*((Head!L18-Head!K18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N19" s="1">
-        <f>'K values'!M18*((Head!M18-Head!L18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M18)+(1/'K values'!L18)))*((Head!M18-Head!L18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O19" s="1">
-        <f>'K values'!N18*((Head!N18-Head!M18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N18)+(1/'K values'!M18)))*((Head!N18-Head!M18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P19" s="1">
-        <f>'K values'!O18*((Head!O18-Head!N18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O18)+(1/'K values'!N18)))*((Head!O18-Head!N18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q19" s="1">
-        <f>'K values'!P18*((Head!P18-Head!O18)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P18)+(1/'K values'!O18)))*((Head!P18-Head!O18)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R19" s="1">
-        <f>'K values'!Q18*((Head!Q18-Head!P18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q18)+(1/'K values'!P18)))*((Head!Q18-Head!P18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S19" s="1">
-        <f>'K values'!R18*((Head!R18-Head!Q18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R18)+(1/'K values'!Q18)))*((Head!R18-Head!Q18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T19" s="1">
-        <f>'K values'!S18*((Head!S18-Head!R18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S18)+(1/'K values'!R18)))*((Head!S18-Head!R18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U19" s="1">
-        <f>'K values'!T18*((Head!T18-Head!S18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T18)+(1/'K values'!S18)))*((Head!T18-Head!S18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V19" s="1">
-        <f>'K values'!U18*((Head!U18-Head!T18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U18)+(1/'K values'!T18)))*((Head!U18-Head!T18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W19" s="1">
-        <f>'K values'!V18*((Head!V18-Head!U18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V18)+(1/'K values'!U18)))*((Head!V18-Head!U18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X19" s="1">
-        <f>'K values'!W18*((Head!W18-Head!V18)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W18)+(1/'K values'!V18)))*((Head!W18-Head!V18)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y19" s="1">
-        <f>'K values'!X18*((Head!X18-Head!W18)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X18)+(1/'K values'!W18)))*((Head!X18-Head!W18)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z19" s="1">
-        <f>'K values'!Y18*((Head!Y18-Head!X18)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y18)+(1/'K values'!X18)))*((Head!Y18-Head!X18)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA19">
         <v>1700</v>
@@ -25961,104 +25962,104 @@
         <v>1800</v>
       </c>
       <c r="B20" s="1">
-        <f>-1*'K values'!A19*((Head!A19)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A19)+(1/'K values'!A19)))*((Head!A19-Head!A19)/100))</f>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f>'K values'!B19*((Head!B19-Head!A19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B19)+(1/'K values'!A19)))*((Head!B19-Head!A19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D20" s="1">
-        <f>'K values'!C19*((Head!C19-Head!B19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C19)+(1/'K values'!B19)))*((Head!C19-Head!B19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E20" s="1">
-        <f>'K values'!D19*((Head!D19-Head!C19)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D19)+(1/'K values'!C19)))*((Head!D19-Head!C19)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>'K values'!E19*((Head!E19-Head!D19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E19)+(1/'K values'!D19)))*((Head!E19-Head!D19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G20" s="1">
-        <f>'K values'!F19*((Head!F19-Head!E19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F19)+(1/'K values'!E19)))*((Head!F19-Head!E19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H20" s="1">
-        <f>'K values'!G19*((Head!G19-Head!F19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G19)+(1/'K values'!F19)))*((Head!G19-Head!F19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I20" s="1">
-        <f>'K values'!H19*((Head!H19-Head!G19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H19)+(1/'K values'!G19)))*((Head!H19-Head!G19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J20" s="1">
-        <f>'K values'!I19*((Head!I19-Head!H19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I19)+(1/'K values'!H19)))*((Head!I19-Head!H19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K20" s="1">
-        <f>'K values'!J19*((Head!J19-Head!I19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J19)+(1/'K values'!I19)))*((Head!J19-Head!I19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L20" s="1">
-        <f>'K values'!K19*((Head!K19-Head!J19)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K19)+(1/'K values'!J19)))*((Head!K19-Head!J19)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M20" s="1">
-        <f>'K values'!L19*((Head!L19-Head!K19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L19)+(1/'K values'!K19)))*((Head!L19-Head!K19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N20" s="1">
-        <f>'K values'!M19*((Head!M19-Head!L19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M19)+(1/'K values'!L19)))*((Head!M19-Head!L19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O20" s="1">
-        <f>'K values'!N19*((Head!N19-Head!M19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N19)+(1/'K values'!M19)))*((Head!N19-Head!M19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P20" s="1">
-        <f>'K values'!O19*((Head!O19-Head!N19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O19)+(1/'K values'!N19)))*((Head!O19-Head!N19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q20" s="1">
-        <f>'K values'!P19*((Head!P19-Head!O19)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P19)+(1/'K values'!O19)))*((Head!P19-Head!O19)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R20" s="1">
-        <f>'K values'!Q19*((Head!Q19-Head!P19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q19)+(1/'K values'!P19)))*((Head!Q19-Head!P19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S20" s="1">
-        <f>'K values'!R19*((Head!R19-Head!Q19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R19)+(1/'K values'!Q19)))*((Head!R19-Head!Q19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T20" s="1">
-        <f>'K values'!S19*((Head!S19-Head!R19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S19)+(1/'K values'!R19)))*((Head!S19-Head!R19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U20" s="1">
-        <f>'K values'!T19*((Head!T19-Head!S19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T19)+(1/'K values'!S19)))*((Head!T19-Head!S19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V20" s="1">
-        <f>'K values'!U19*((Head!U19-Head!T19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U19)+(1/'K values'!T19)))*((Head!U19-Head!T19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W20" s="1">
-        <f>'K values'!V19*((Head!V19-Head!U19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V19)+(1/'K values'!U19)))*((Head!V19-Head!U19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X20" s="1">
-        <f>'K values'!W19*((Head!W19-Head!V19)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W19)+(1/'K values'!V19)))*((Head!W19-Head!V19)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y20" s="1">
-        <f>'K values'!X19*((Head!X19-Head!W19)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X19)+(1/'K values'!W19)))*((Head!X19-Head!W19)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z20" s="1">
-        <f>'K values'!Y19*((Head!Y19-Head!X19)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y19)+(1/'K values'!X19)))*((Head!Y19-Head!X19)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA20">
         <v>1800</v>
@@ -26069,104 +26070,104 @@
         <v>1900</v>
       </c>
       <c r="B21" s="1">
-        <f>-1*'K values'!A20*((Head!A20)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A20)+(1/'K values'!A20)))*((Head!A20-Head!A20)/100))</f>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
-        <f>'K values'!B20*((Head!B20-Head!A20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B20)+(1/'K values'!A20)))*((Head!B20-Head!A20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D21" s="1">
-        <f>'K values'!C20*((Head!C20-Head!B20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C20)+(1/'K values'!B20)))*((Head!C20-Head!B20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E21" s="1">
-        <f>'K values'!D20*((Head!D20-Head!C20)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D20)+(1/'K values'!C20)))*((Head!D20-Head!C20)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>'K values'!E20*((Head!E20-Head!D20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E20)+(1/'K values'!D20)))*((Head!E20-Head!D20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G21" s="1">
-        <f>'K values'!F20*((Head!F20-Head!E20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F20)+(1/'K values'!E20)))*((Head!F20-Head!E20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H21" s="1">
-        <f>'K values'!G20*((Head!G20-Head!F20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G20)+(1/'K values'!F20)))*((Head!G20-Head!F20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I21" s="1">
-        <f>'K values'!H20*((Head!H20-Head!G20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H20)+(1/'K values'!G20)))*((Head!H20-Head!G20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J21" s="1">
-        <f>'K values'!I20*((Head!I20-Head!H20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I20)+(1/'K values'!H20)))*((Head!I20-Head!H20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K21" s="1">
-        <f>'K values'!J20*((Head!J20-Head!I20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J20)+(1/'K values'!I20)))*((Head!J20-Head!I20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L21" s="1">
-        <f>'K values'!K20*((Head!K20-Head!J20)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K20)+(1/'K values'!J20)))*((Head!K20-Head!J20)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M21" s="1">
-        <f>'K values'!L20*((Head!L20-Head!K20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L20)+(1/'K values'!K20)))*((Head!L20-Head!K20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N21" s="1">
-        <f>'K values'!M20*((Head!M20-Head!L20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M20)+(1/'K values'!L20)))*((Head!M20-Head!L20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O21" s="1">
-        <f>'K values'!N20*((Head!N20-Head!M20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N20)+(1/'K values'!M20)))*((Head!N20-Head!M20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P21" s="1">
-        <f>'K values'!O20*((Head!O20-Head!N20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O20)+(1/'K values'!N20)))*((Head!O20-Head!N20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q21" s="1">
-        <f>'K values'!P20*((Head!P20-Head!O20)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P20)+(1/'K values'!O20)))*((Head!P20-Head!O20)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R21" s="1">
-        <f>'K values'!Q20*((Head!Q20-Head!P20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q20)+(1/'K values'!P20)))*((Head!Q20-Head!P20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S21" s="1">
-        <f>'K values'!R20*((Head!R20-Head!Q20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R20)+(1/'K values'!Q20)))*((Head!R20-Head!Q20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T21" s="1">
-        <f>'K values'!S20*((Head!S20-Head!R20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S20)+(1/'K values'!R20)))*((Head!S20-Head!R20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U21" s="1">
-        <f>'K values'!T20*((Head!T20-Head!S20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T20)+(1/'K values'!S20)))*((Head!T20-Head!S20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V21" s="1">
-        <f>'K values'!U20*((Head!U20-Head!T20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U20)+(1/'K values'!T20)))*((Head!U20-Head!T20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W21" s="1">
-        <f>'K values'!V20*((Head!V20-Head!U20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V20)+(1/'K values'!U20)))*((Head!V20-Head!U20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X21" s="1">
-        <f>'K values'!W20*((Head!W20-Head!V20)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W20)+(1/'K values'!V20)))*((Head!W20-Head!V20)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y21" s="1">
-        <f>'K values'!X20*((Head!X20-Head!W20)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X20)+(1/'K values'!W20)))*((Head!X20-Head!W20)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z21" s="1">
-        <f>'K values'!Y20*((Head!Y20-Head!X20)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y20)+(1/'K values'!X20)))*((Head!Y20-Head!X20)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA21">
         <v>1900</v>
@@ -26177,104 +26178,104 @@
         <v>2000</v>
       </c>
       <c r="B22" s="1">
-        <f>-1*'K values'!A21*((Head!A21)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A21)+(1/'K values'!A21)))*((Head!A21-Head!A21)/100))</f>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <f>'K values'!B21*((Head!B21-Head!A21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B21)+(1/'K values'!A21)))*((Head!B21-Head!A21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D22" s="1">
-        <f>'K values'!C21*((Head!C21-Head!B21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C21)+(1/'K values'!B21)))*((Head!C21-Head!B21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E22" s="1">
-        <f>'K values'!D21*((Head!D21-Head!C21)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D21)+(1/'K values'!C21)))*((Head!D21-Head!C21)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>'K values'!E21*((Head!E21-Head!D21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E21)+(1/'K values'!D21)))*((Head!E21-Head!D21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G22" s="1">
-        <f>'K values'!F21*((Head!F21-Head!E21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F21)+(1/'K values'!E21)))*((Head!F21-Head!E21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H22" s="1">
-        <f>'K values'!G21*((Head!G21-Head!F21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G21)+(1/'K values'!F21)))*((Head!G21-Head!F21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I22" s="1">
-        <f>'K values'!H21*((Head!H21-Head!G21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H21)+(1/'K values'!G21)))*((Head!H21-Head!G21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J22" s="1">
-        <f>'K values'!I21*((Head!I21-Head!H21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I21)+(1/'K values'!H21)))*((Head!I21-Head!H21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K22" s="1">
-        <f>'K values'!J21*((Head!J21-Head!I21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J21)+(1/'K values'!I21)))*((Head!J21-Head!I21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L22" s="1">
-        <f>'K values'!K21*((Head!K21-Head!J21)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K21)+(1/'K values'!J21)))*((Head!K21-Head!J21)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M22" s="1">
-        <f>'K values'!L21*((Head!L21-Head!K21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L21)+(1/'K values'!K21)))*((Head!L21-Head!K21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N22" s="1">
-        <f>'K values'!M21*((Head!M21-Head!L21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M21)+(1/'K values'!L21)))*((Head!M21-Head!L21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O22" s="1">
-        <f>'K values'!N21*((Head!N21-Head!M21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N21)+(1/'K values'!M21)))*((Head!N21-Head!M21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P22" s="1">
-        <f>'K values'!O21*((Head!O21-Head!N21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O21)+(1/'K values'!N21)))*((Head!O21-Head!N21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q22" s="1">
-        <f>'K values'!P21*((Head!P21-Head!O21)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P21)+(1/'K values'!O21)))*((Head!P21-Head!O21)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R22" s="1">
-        <f>'K values'!Q21*((Head!Q21-Head!P21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q21)+(1/'K values'!P21)))*((Head!Q21-Head!P21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S22" s="1">
-        <f>'K values'!R21*((Head!R21-Head!Q21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R21)+(1/'K values'!Q21)))*((Head!R21-Head!Q21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T22" s="1">
-        <f>'K values'!S21*((Head!S21-Head!R21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S21)+(1/'K values'!R21)))*((Head!S21-Head!R21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U22" s="1">
-        <f>'K values'!T21*((Head!T21-Head!S21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T21)+(1/'K values'!S21)))*((Head!T21-Head!S21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V22" s="1">
-        <f>'K values'!U21*((Head!U21-Head!T21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U21)+(1/'K values'!T21)))*((Head!U21-Head!T21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W22" s="1">
-        <f>'K values'!V21*((Head!V21-Head!U21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V21)+(1/'K values'!U21)))*((Head!V21-Head!U21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X22" s="1">
-        <f>'K values'!W21*((Head!W21-Head!V21)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W21)+(1/'K values'!V21)))*((Head!W21-Head!V21)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y22" s="1">
-        <f>'K values'!X21*((Head!X21-Head!W21)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X21)+(1/'K values'!W21)))*((Head!X21-Head!W21)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z22" s="1">
-        <f>'K values'!Y21*((Head!Y21-Head!X21)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y21)+(1/'K values'!X21)))*((Head!Y21-Head!X21)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA22">
         <v>2000</v>
@@ -26285,104 +26286,104 @@
         <v>2100</v>
       </c>
       <c r="B23" s="1">
-        <f>-1*'K values'!A22*((Head!A22)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A22)+(1/'K values'!A22)))*((Head!A22-Head!A22)/100))</f>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
-        <f>'K values'!B22*((Head!B22-Head!A22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B22)+(1/'K values'!A22)))*((Head!B22-Head!A22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D23" s="1">
-        <f>'K values'!C22*((Head!C22-Head!B22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C22)+(1/'K values'!B22)))*((Head!C22-Head!B22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E23" s="1">
-        <f>'K values'!D22*((Head!D22-Head!C22)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D22)+(1/'K values'!C22)))*((Head!D22-Head!C22)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>'K values'!E22*((Head!E22-Head!D22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E22)+(1/'K values'!D22)))*((Head!E22-Head!D22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G23" s="1">
-        <f>'K values'!F22*((Head!F22-Head!E22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F22)+(1/'K values'!E22)))*((Head!F22-Head!E22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H23" s="1">
-        <f>'K values'!G22*((Head!G22-Head!F22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G22)+(1/'K values'!F22)))*((Head!G22-Head!F22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I23" s="1">
-        <f>'K values'!H22*((Head!H22-Head!G22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H22)+(1/'K values'!G22)))*((Head!H22-Head!G22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J23" s="1">
-        <f>'K values'!I22*((Head!I22-Head!H22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I22)+(1/'K values'!H22)))*((Head!I22-Head!H22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K23" s="1">
-        <f>'K values'!J22*((Head!J22-Head!I22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J22)+(1/'K values'!I22)))*((Head!J22-Head!I22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L23" s="1">
-        <f>'K values'!K22*((Head!K22-Head!J22)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K22)+(1/'K values'!J22)))*((Head!K22-Head!J22)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M23" s="1">
-        <f>'K values'!L22*((Head!L22-Head!K22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L22)+(1/'K values'!K22)))*((Head!L22-Head!K22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N23" s="1">
-        <f>'K values'!M22*((Head!M22-Head!L22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M22)+(1/'K values'!L22)))*((Head!M22-Head!L22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O23" s="1">
-        <f>'K values'!N22*((Head!N22-Head!M22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N22)+(1/'K values'!M22)))*((Head!N22-Head!M22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P23" s="1">
-        <f>'K values'!O22*((Head!O22-Head!N22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O22)+(1/'K values'!N22)))*((Head!O22-Head!N22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q23" s="1">
-        <f>'K values'!P22*((Head!P22-Head!O22)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P22)+(1/'K values'!O22)))*((Head!P22-Head!O22)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R23" s="1">
-        <f>'K values'!Q22*((Head!Q22-Head!P22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q22)+(1/'K values'!P22)))*((Head!Q22-Head!P22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S23" s="1">
-        <f>'K values'!R22*((Head!R22-Head!Q22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R22)+(1/'K values'!Q22)))*((Head!R22-Head!Q22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T23" s="1">
-        <f>'K values'!S22*((Head!S22-Head!R22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S22)+(1/'K values'!R22)))*((Head!S22-Head!R22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U23" s="1">
-        <f>'K values'!T22*((Head!T22-Head!S22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T22)+(1/'K values'!S22)))*((Head!T22-Head!S22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V23" s="1">
-        <f>'K values'!U22*((Head!U22-Head!T22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U22)+(1/'K values'!T22)))*((Head!U22-Head!T22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W23" s="1">
-        <f>'K values'!V22*((Head!V22-Head!U22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V22)+(1/'K values'!U22)))*((Head!V22-Head!U22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X23" s="1">
-        <f>'K values'!W22*((Head!W22-Head!V22)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W22)+(1/'K values'!V22)))*((Head!W22-Head!V22)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y23" s="1">
-        <f>'K values'!X22*((Head!X22-Head!W22)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X22)+(1/'K values'!W22)))*((Head!X22-Head!W22)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z23" s="1">
-        <f>'K values'!Y22*((Head!Y22-Head!X22)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y22)+(1/'K values'!X22)))*((Head!Y22-Head!X22)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA23">
         <v>2100</v>
@@ -26393,104 +26394,104 @@
         <v>2200</v>
       </c>
       <c r="B24" s="1">
-        <f>-1*'K values'!A23*((Head!A23)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A23)+(1/'K values'!A23)))*((Head!A23-Head!A23)/100))</f>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <f>'K values'!B23*((Head!B23-Head!A23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B23)+(1/'K values'!A23)))*((Head!B23-Head!A23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D24" s="1">
-        <f>'K values'!C23*((Head!C23-Head!B23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C23)+(1/'K values'!B23)))*((Head!C23-Head!B23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E24" s="1">
-        <f>'K values'!D23*((Head!D23-Head!C23)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D23)+(1/'K values'!C23)))*((Head!D23-Head!C23)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>'K values'!E23*((Head!E23-Head!D23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E23)+(1/'K values'!D23)))*((Head!E23-Head!D23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G24" s="1">
-        <f>'K values'!F23*((Head!F23-Head!E23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F23)+(1/'K values'!E23)))*((Head!F23-Head!E23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H24" s="1">
-        <f>'K values'!G23*((Head!G23-Head!F23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G23)+(1/'K values'!F23)))*((Head!G23-Head!F23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I24" s="1">
-        <f>'K values'!H23*((Head!H23-Head!G23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H23)+(1/'K values'!G23)))*((Head!H23-Head!G23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J24" s="1">
-        <f>'K values'!I23*((Head!I23-Head!H23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I23)+(1/'K values'!H23)))*((Head!I23-Head!H23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K24" s="1">
-        <f>'K values'!J23*((Head!J23-Head!I23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J23)+(1/'K values'!I23)))*((Head!J23-Head!I23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L24" s="1">
-        <f>'K values'!K23*((Head!K23-Head!J23)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K23)+(1/'K values'!J23)))*((Head!K23-Head!J23)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M24" s="1">
-        <f>'K values'!L23*((Head!L23-Head!K23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L23)+(1/'K values'!K23)))*((Head!L23-Head!K23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N24" s="1">
-        <f>'K values'!M23*((Head!M23-Head!L23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M23)+(1/'K values'!L23)))*((Head!M23-Head!L23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O24" s="1">
-        <f>'K values'!N23*((Head!N23-Head!M23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N23)+(1/'K values'!M23)))*((Head!N23-Head!M23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P24" s="1">
-        <f>'K values'!O23*((Head!O23-Head!N23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O23)+(1/'K values'!N23)))*((Head!O23-Head!N23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q24" s="1">
-        <f>'K values'!P23*((Head!P23-Head!O23)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P23)+(1/'K values'!O23)))*((Head!P23-Head!O23)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R24" s="1">
-        <f>'K values'!Q23*((Head!Q23-Head!P23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q23)+(1/'K values'!P23)))*((Head!Q23-Head!P23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S24" s="1">
-        <f>'K values'!R23*((Head!R23-Head!Q23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R23)+(1/'K values'!Q23)))*((Head!R23-Head!Q23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T24" s="1">
-        <f>'K values'!S23*((Head!S23-Head!R23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S23)+(1/'K values'!R23)))*((Head!S23-Head!R23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U24" s="1">
-        <f>'K values'!T23*((Head!T23-Head!S23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T23)+(1/'K values'!S23)))*((Head!T23-Head!S23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V24" s="1">
-        <f>'K values'!U23*((Head!U23-Head!T23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U23)+(1/'K values'!T23)))*((Head!U23-Head!T23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W24" s="1">
-        <f>'K values'!V23*((Head!V23-Head!U23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V23)+(1/'K values'!U23)))*((Head!V23-Head!U23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X24" s="1">
-        <f>'K values'!W23*((Head!W23-Head!V23)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W23)+(1/'K values'!V23)))*((Head!W23-Head!V23)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y24" s="1">
-        <f>'K values'!X23*((Head!X23-Head!W23)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X23)+(1/'K values'!W23)))*((Head!X23-Head!W23)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z24" s="1">
-        <f>'K values'!Y23*((Head!Y23-Head!X23)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y23)+(1/'K values'!X23)))*((Head!Y23-Head!X23)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA24">
         <v>2200</v>
@@ -26501,104 +26502,104 @@
         <v>2300</v>
       </c>
       <c r="B25" s="1">
-        <f>-1*'K values'!A24*((Head!A24)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A24)+(1/'K values'!A24)))*((Head!A24-Head!A24)/100))</f>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
-        <f>'K values'!B24*((Head!B24-Head!A24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B24)+(1/'K values'!A24)))*((Head!B24-Head!A24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D25" s="1">
-        <f>'K values'!C24*((Head!C24-Head!B24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C24)+(1/'K values'!B24)))*((Head!C24-Head!B24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E25" s="1">
-        <f>'K values'!D24*((Head!D24-Head!C24)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D24)+(1/'K values'!C24)))*((Head!D24-Head!C24)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>'K values'!E24*((Head!E24-Head!D24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E24)+(1/'K values'!D24)))*((Head!E24-Head!D24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G25" s="1">
-        <f>'K values'!F24*((Head!F24-Head!E24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F24)+(1/'K values'!E24)))*((Head!F24-Head!E24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H25" s="1">
-        <f>'K values'!G24*((Head!G24-Head!F24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G24)+(1/'K values'!F24)))*((Head!G24-Head!F24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I25" s="1">
-        <f>'K values'!H24*((Head!H24-Head!G24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H24)+(1/'K values'!G24)))*((Head!H24-Head!G24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J25" s="1">
-        <f>'K values'!I24*((Head!I24-Head!H24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I24)+(1/'K values'!H24)))*((Head!I24-Head!H24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K25" s="1">
-        <f>'K values'!J24*((Head!J24-Head!I24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J24)+(1/'K values'!I24)))*((Head!J24-Head!I24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L25" s="1">
-        <f>'K values'!K24*((Head!K24-Head!J24)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K24)+(1/'K values'!J24)))*((Head!K24-Head!J24)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M25" s="1">
-        <f>'K values'!L24*((Head!L24-Head!K24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L24)+(1/'K values'!K24)))*((Head!L24-Head!K24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N25" s="1">
-        <f>'K values'!M24*((Head!M24-Head!L24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M24)+(1/'K values'!L24)))*((Head!M24-Head!L24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O25" s="1">
-        <f>'K values'!N24*((Head!N24-Head!M24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N24)+(1/'K values'!M24)))*((Head!N24-Head!M24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P25" s="1">
-        <f>'K values'!O24*((Head!O24-Head!N24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O24)+(1/'K values'!N24)))*((Head!O24-Head!N24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q25" s="1">
-        <f>'K values'!P24*((Head!P24-Head!O24)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P24)+(1/'K values'!O24)))*((Head!P24-Head!O24)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R25" s="1">
-        <f>'K values'!Q24*((Head!Q24-Head!P24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q24)+(1/'K values'!P24)))*((Head!Q24-Head!P24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S25" s="1">
-        <f>'K values'!R24*((Head!R24-Head!Q24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R24)+(1/'K values'!Q24)))*((Head!R24-Head!Q24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T25" s="1">
-        <f>'K values'!S24*((Head!S24-Head!R24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S24)+(1/'K values'!R24)))*((Head!S24-Head!R24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U25" s="1">
-        <f>'K values'!T24*((Head!T24-Head!S24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T24)+(1/'K values'!S24)))*((Head!T24-Head!S24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V25" s="1">
-        <f>'K values'!U24*((Head!U24-Head!T24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U24)+(1/'K values'!T24)))*((Head!U24-Head!T24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W25" s="1">
-        <f>'K values'!V24*((Head!V24-Head!U24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V24)+(1/'K values'!U24)))*((Head!V24-Head!U24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X25" s="1">
-        <f>'K values'!W24*((Head!W24-Head!V24)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W24)+(1/'K values'!V24)))*((Head!W24-Head!V24)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y25" s="1">
-        <f>'K values'!X24*((Head!X24-Head!W24)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X24)+(1/'K values'!W24)))*((Head!X24-Head!W24)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z25" s="1">
-        <f>'K values'!Y24*((Head!Y24-Head!X24)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y24)+(1/'K values'!X24)))*((Head!Y24-Head!X24)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA25">
         <v>2300</v>
@@ -26609,104 +26610,104 @@
         <v>2400</v>
       </c>
       <c r="B26" s="1">
-        <f>-1*'K values'!A25*((Head!A25)/100)</f>
-        <v>-0.15</v>
+        <f>-((2/((1/'K values'!A25)+(1/'K values'!A25)))*((Head!A25-Head!A25)/100))</f>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
-        <f>'K values'!B25*((Head!B25-Head!A25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!B25)+(1/'K values'!A25)))*((Head!B25-Head!A25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="D26" s="1">
-        <f>'K values'!C25*((Head!C25-Head!B25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!C25)+(1/'K values'!B25)))*((Head!C25-Head!B25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="E26" s="1">
-        <f>'K values'!D25*((Head!D25-Head!C25)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!D25)+(1/'K values'!C25)))*((Head!D25-Head!C25)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>'K values'!E25*((Head!E25-Head!D25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!E25)+(1/'K values'!D25)))*((Head!E25-Head!D25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="G26" s="1">
-        <f>'K values'!F25*((Head!F25-Head!E25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!F25)+(1/'K values'!E25)))*((Head!F25-Head!E25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="H26" s="1">
-        <f>'K values'!G25*((Head!G25-Head!F25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!G25)+(1/'K values'!F25)))*((Head!G25-Head!F25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="I26" s="1">
-        <f>'K values'!H25*((Head!H25-Head!G25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!H25)+(1/'K values'!G25)))*((Head!H25-Head!G25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="J26" s="1">
-        <f>'K values'!I25*((Head!I25-Head!H25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!I25)+(1/'K values'!H25)))*((Head!I25-Head!H25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="K26" s="1">
-        <f>'K values'!J25*((Head!J25-Head!I25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!J25)+(1/'K values'!I25)))*((Head!J25-Head!I25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="L26" s="1">
-        <f>'K values'!K25*((Head!K25-Head!J25)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!K25)+(1/'K values'!J25)))*((Head!K25-Head!J25)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="M26" s="1">
-        <f>'K values'!L25*((Head!L25-Head!K25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!L25)+(1/'K values'!K25)))*((Head!L25-Head!K25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="N26" s="1">
-        <f>'K values'!M25*((Head!M25-Head!L25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!M25)+(1/'K values'!L25)))*((Head!M25-Head!L25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="O26" s="1">
-        <f>'K values'!N25*((Head!N25-Head!M25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!N25)+(1/'K values'!M25)))*((Head!N25-Head!M25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="P26" s="1">
-        <f>'K values'!O25*((Head!O25-Head!N25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!O25)+(1/'K values'!N25)))*((Head!O25-Head!N25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Q26" s="1">
-        <f>'K values'!P25*((Head!P25-Head!O25)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!P25)+(1/'K values'!O25)))*((Head!P25-Head!O25)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="R26" s="1">
-        <f>'K values'!Q25*((Head!Q25-Head!P25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Q25)+(1/'K values'!P25)))*((Head!Q25-Head!P25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="S26" s="1">
-        <f>'K values'!R25*((Head!R25-Head!Q25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!R25)+(1/'K values'!Q25)))*((Head!R25-Head!Q25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="T26" s="1">
-        <f>'K values'!S25*((Head!S25-Head!R25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!S25)+(1/'K values'!R25)))*((Head!S25-Head!R25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="U26" s="1">
-        <f>'K values'!T25*((Head!T25-Head!S25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!T25)+(1/'K values'!S25)))*((Head!T25-Head!S25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="V26" s="1">
-        <f>'K values'!U25*((Head!U25-Head!T25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!U25)+(1/'K values'!T25)))*((Head!U25-Head!T25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="W26" s="1">
-        <f>'K values'!V25*((Head!V25-Head!U25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!V25)+(1/'K values'!U25)))*((Head!V25-Head!U25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="X26" s="1">
-        <f>'K values'!W25*((Head!W25-Head!V25)/100)</f>
-        <v>-1.9999999999999931E-3</v>
+        <f>-((2/((1/'K values'!W25)+(1/'K values'!V25)))*((Head!W25-Head!V25)/100))</f>
+        <v>1.9999999999999931E-3</v>
       </c>
       <c r="Y26" s="1">
-        <f>'K values'!X25*((Head!X25-Head!W25)/100)</f>
-        <v>-2.0999999999999908E-3</v>
+        <f>-((2/((1/'K values'!X25)+(1/'K values'!W25)))*((Head!X25-Head!W25)/100))</f>
+        <v>2.0999999999999908E-3</v>
       </c>
       <c r="Z26" s="1">
-        <f>'K values'!Y25*((Head!Y25-Head!X25)/100)</f>
-        <v>-2.1000000000000085E-3</v>
+        <f>-((2/((1/'K values'!Y25)+(1/'K values'!X25)))*((Head!Y25-Head!X25)/100))</f>
+        <v>2.1000000000000085E-3</v>
       </c>
       <c r="AA26">
         <v>2400</v>
@@ -26717,7 +26718,7 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -26725,7 +26726,7 @@
         <v>100</v>
       </c>
       <c r="B30">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -26733,7 +26734,7 @@
         <v>200</v>
       </c>
       <c r="B31">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -26741,7 +26742,7 @@
         <v>300</v>
       </c>
       <c r="B32">
-        <v>-1.9999999999999931E-3</v>
+        <v>1.9999999999999931E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -26749,7 +26750,7 @@
         <v>400</v>
       </c>
       <c r="B33">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -26757,7 +26758,7 @@
         <v>500</v>
       </c>
       <c r="B34">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -26765,7 +26766,7 @@
         <v>600</v>
       </c>
       <c r="B35">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -26773,7 +26774,7 @@
         <v>700</v>
       </c>
       <c r="B36">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -26781,7 +26782,7 @@
         <v>800</v>
       </c>
       <c r="B37">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -26789,7 +26790,7 @@
         <v>900</v>
       </c>
       <c r="B38">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -26797,7 +26798,7 @@
         <v>1000</v>
       </c>
       <c r="B39">
-        <v>-1.9999999999999931E-3</v>
+        <v>1.9999999999999931E-3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -26805,7 +26806,7 @@
         <v>1100</v>
       </c>
       <c r="B40">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -26813,7 +26814,7 @@
         <v>1200</v>
       </c>
       <c r="B41">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -26821,7 +26822,7 @@
         <v>1300</v>
       </c>
       <c r="B42">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -26829,7 +26830,7 @@
         <v>1400</v>
       </c>
       <c r="B43">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -26837,7 +26838,7 @@
         <v>1500</v>
       </c>
       <c r="B44">
-        <v>-1.9999999999999931E-3</v>
+        <v>1.9999999999999931E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -26845,7 +26846,7 @@
         <v>1600</v>
       </c>
       <c r="B45">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -26853,7 +26854,7 @@
         <v>1700</v>
       </c>
       <c r="B46">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -26861,7 +26862,7 @@
         <v>1800</v>
       </c>
       <c r="B47">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -26869,7 +26870,7 @@
         <v>1900</v>
       </c>
       <c r="B48">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -26877,7 +26878,7 @@
         <v>2000</v>
       </c>
       <c r="B49">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -26885,7 +26886,7 @@
         <v>2100</v>
       </c>
       <c r="B50">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -26893,7 +26894,7 @@
         <v>2200</v>
       </c>
       <c r="B51">
-        <v>-1.9999999999999931E-3</v>
+        <v>1.9999999999999931E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -26901,7 +26902,7 @@
         <v>2300</v>
       </c>
       <c r="B52">
-        <v>-2.0999999999999908E-3</v>
+        <v>2.0999999999999908E-3</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -26909,7 +26910,7 @@
         <v>2400</v>
       </c>
       <c r="B53">
-        <v>-2.1000000000000085E-3</v>
+        <v>2.1000000000000085E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>